<commit_message>
Set year to excel template
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_detail_daily.xlsx
+++ b/public/template/excel/format_laporan_detail_daily.xlsx
@@ -1432,7 +1432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1617,9 +1617,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1638,8 +1635,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2240,7 +2243,7 @@
   <dimension ref="A1:BW465"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="D10" sqref="D10:BT10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2257,49 +2260,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
     </row>
     <row r="2" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="74" t="s">
         <v>279</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="77" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="74" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
       <c r="H7" s="56"/>
     </row>
     <row r="8" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
@@ -2309,521 +2312,381 @@
       <c r="B8" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="78" t="s">
         <v>291</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72" t="s">
+      <c r="D8" s="78"/>
+      <c r="E8" s="78" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72" t="s">
+      <c r="F8" s="78"/>
+      <c r="G8" s="78" t="s">
         <v>293</v>
       </c>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72" t="s">
+      <c r="H8" s="78"/>
+      <c r="I8" s="78" t="s">
         <v>294</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72" t="s">
+      <c r="J8" s="78"/>
+      <c r="K8" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72" t="s">
+      <c r="L8" s="78"/>
+      <c r="M8" s="78" t="s">
         <v>296</v>
       </c>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72" t="s">
+      <c r="N8" s="78"/>
+      <c r="O8" s="78" t="s">
         <v>297</v>
       </c>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72" t="s">
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72" t="s">
+      <c r="R8" s="78"/>
+      <c r="S8" s="78" t="s">
         <v>299</v>
       </c>
-      <c r="T8" s="72"/>
-      <c r="U8" s="72" t="s">
+      <c r="T8" s="78"/>
+      <c r="U8" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72" t="s">
+      <c r="V8" s="78"/>
+      <c r="W8" s="78" t="s">
         <v>301</v>
       </c>
-      <c r="X8" s="72"/>
-      <c r="Y8" s="72" t="s">
+      <c r="X8" s="78"/>
+      <c r="Y8" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="Z8" s="72"/>
-      <c r="AA8" s="72" t="s">
+      <c r="Z8" s="78"/>
+      <c r="AA8" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="72" t="s">
+      <c r="AB8" s="78"/>
+      <c r="AC8" s="78" t="s">
         <v>304</v>
       </c>
-      <c r="AD8" s="72"/>
-      <c r="AE8" s="72" t="s">
+      <c r="AD8" s="78"/>
+      <c r="AE8" s="78" t="s">
         <v>305</v>
       </c>
-      <c r="AF8" s="72"/>
-      <c r="AG8" s="72" t="s">
+      <c r="AF8" s="78"/>
+      <c r="AG8" s="78" t="s">
         <v>306</v>
       </c>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="72" t="s">
+      <c r="AH8" s="78"/>
+      <c r="AI8" s="78" t="s">
         <v>307</v>
       </c>
-      <c r="AJ8" s="72"/>
-      <c r="AK8" s="72" t="s">
+      <c r="AJ8" s="78"/>
+      <c r="AK8" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="AL8" s="72"/>
-      <c r="AM8" s="72" t="s">
+      <c r="AL8" s="78"/>
+      <c r="AM8" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="AN8" s="72"/>
-      <c r="AO8" s="72" t="s">
+      <c r="AN8" s="78"/>
+      <c r="AO8" s="78" t="s">
         <v>310</v>
       </c>
-      <c r="AP8" s="72"/>
-      <c r="AQ8" s="72" t="s">
+      <c r="AP8" s="78"/>
+      <c r="AQ8" s="78" t="s">
         <v>311</v>
       </c>
-      <c r="AR8" s="72"/>
-      <c r="AS8" s="72" t="s">
+      <c r="AR8" s="78"/>
+      <c r="AS8" s="78" t="s">
         <v>312</v>
       </c>
-      <c r="AT8" s="72"/>
-      <c r="AU8" s="72" t="s">
+      <c r="AT8" s="78"/>
+      <c r="AU8" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="AV8" s="72"/>
-      <c r="AW8" s="72" t="s">
+      <c r="AV8" s="78"/>
+      <c r="AW8" s="78" t="s">
         <v>314</v>
       </c>
-      <c r="AX8" s="72"/>
-      <c r="AY8" s="72" t="s">
+      <c r="AX8" s="78"/>
+      <c r="AY8" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="AZ8" s="72"/>
-      <c r="BA8" s="72" t="s">
+      <c r="AZ8" s="78"/>
+      <c r="BA8" s="78" t="s">
         <v>316</v>
       </c>
-      <c r="BB8" s="72"/>
-      <c r="BC8" s="73" t="s">
+      <c r="BB8" s="78"/>
+      <c r="BC8" s="80" t="s">
         <v>317</v>
       </c>
-      <c r="BD8" s="73"/>
-      <c r="BE8" s="72" t="s">
+      <c r="BD8" s="80"/>
+      <c r="BE8" s="78" t="s">
         <v>318</v>
       </c>
-      <c r="BF8" s="72"/>
-      <c r="BG8" s="72" t="s">
+      <c r="BF8" s="78"/>
+      <c r="BG8" s="78" t="s">
         <v>319</v>
       </c>
-      <c r="BH8" s="72"/>
-      <c r="BI8" s="72" t="s">
+      <c r="BH8" s="78"/>
+      <c r="BI8" s="78" t="s">
         <v>320</v>
       </c>
-      <c r="BJ8" s="72"/>
-      <c r="BK8" s="72" t="s">
+      <c r="BJ8" s="78"/>
+      <c r="BK8" s="78" t="s">
         <v>321</v>
       </c>
-      <c r="BL8" s="72"/>
-      <c r="BM8" s="72" t="s">
+      <c r="BL8" s="78"/>
+      <c r="BM8" s="78" t="s">
         <v>322</v>
       </c>
-      <c r="BN8" s="72"/>
-      <c r="BO8" s="72" t="s">
+      <c r="BN8" s="78"/>
+      <c r="BO8" s="78" t="s">
         <v>323</v>
       </c>
-      <c r="BP8" s="72"/>
-      <c r="BQ8" s="72" t="s">
+      <c r="BP8" s="78"/>
+      <c r="BQ8" s="78" t="s">
         <v>324</v>
       </c>
-      <c r="BR8" s="72"/>
-      <c r="BS8" s="72" t="s">
+      <c r="BR8" s="78"/>
+      <c r="BS8" s="78" t="s">
         <v>325</v>
       </c>
-      <c r="BT8" s="72"/>
-      <c r="BU8" s="72"/>
-      <c r="BV8" s="72"/>
-      <c r="BW8" s="72" t="s">
+      <c r="BT8" s="78"/>
+      <c r="BU8" s="78"/>
+      <c r="BV8" s="78"/>
+      <c r="BW8" s="78" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="79"/>
       <c r="B9" s="79"/>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72" t="s">
+      <c r="D9" s="78"/>
+      <c r="E9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72" t="s">
+      <c r="F9" s="78"/>
+      <c r="G9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72" t="s">
+      <c r="H9" s="78"/>
+      <c r="I9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72" t="s">
+      <c r="J9" s="78"/>
+      <c r="K9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72" t="s">
+      <c r="L9" s="78"/>
+      <c r="M9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="N9" s="72"/>
-      <c r="O9" s="72" t="s">
+      <c r="N9" s="78"/>
+      <c r="O9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="P9" s="72"/>
-      <c r="Q9" s="72" t="s">
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="R9" s="72"/>
-      <c r="S9" s="72" t="s">
+      <c r="R9" s="78"/>
+      <c r="S9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="T9" s="72"/>
-      <c r="U9" s="72" t="s">
+      <c r="T9" s="78"/>
+      <c r="U9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="V9" s="72"/>
-      <c r="W9" s="72" t="s">
+      <c r="V9" s="78"/>
+      <c r="W9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="X9" s="72"/>
-      <c r="Y9" s="72" t="s">
+      <c r="X9" s="78"/>
+      <c r="Y9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="Z9" s="72"/>
-      <c r="AA9" s="72" t="s">
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AB9" s="72"/>
-      <c r="AC9" s="72" t="s">
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AD9" s="72"/>
-      <c r="AE9" s="72" t="s">
+      <c r="AD9" s="78"/>
+      <c r="AE9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AF9" s="72"/>
-      <c r="AG9" s="72" t="s">
+      <c r="AF9" s="78"/>
+      <c r="AG9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AH9" s="72"/>
-      <c r="AI9" s="72" t="s">
+      <c r="AH9" s="78"/>
+      <c r="AI9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AJ9" s="72"/>
-      <c r="AK9" s="72" t="s">
+      <c r="AJ9" s="78"/>
+      <c r="AK9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AL9" s="72"/>
-      <c r="AM9" s="72" t="s">
+      <c r="AL9" s="78"/>
+      <c r="AM9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AN9" s="72"/>
-      <c r="AO9" s="72" t="s">
+      <c r="AN9" s="78"/>
+      <c r="AO9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AP9" s="72"/>
-      <c r="AQ9" s="72" t="s">
+      <c r="AP9" s="78"/>
+      <c r="AQ9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AR9" s="72"/>
-      <c r="AS9" s="72" t="s">
+      <c r="AR9" s="78"/>
+      <c r="AS9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AT9" s="72"/>
-      <c r="AU9" s="72" t="s">
+      <c r="AT9" s="78"/>
+      <c r="AU9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AV9" s="72"/>
-      <c r="AW9" s="72" t="s">
+      <c r="AV9" s="78"/>
+      <c r="AW9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AX9" s="72"/>
-      <c r="AY9" s="72" t="s">
+      <c r="AX9" s="78"/>
+      <c r="AY9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="AZ9" s="72"/>
-      <c r="BA9" s="72" t="s">
+      <c r="AZ9" s="78"/>
+      <c r="BA9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BB9" s="72"/>
-      <c r="BC9" s="73" t="s">
+      <c r="BB9" s="78"/>
+      <c r="BC9" s="80" t="s">
         <v>168</v>
       </c>
-      <c r="BD9" s="73"/>
-      <c r="BE9" s="72" t="s">
+      <c r="BD9" s="80"/>
+      <c r="BE9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BF9" s="72"/>
-      <c r="BG9" s="72" t="s">
+      <c r="BF9" s="78"/>
+      <c r="BG9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BH9" s="72"/>
-      <c r="BI9" s="72" t="s">
+      <c r="BH9" s="78"/>
+      <c r="BI9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BJ9" s="72"/>
-      <c r="BK9" s="72" t="s">
+      <c r="BJ9" s="78"/>
+      <c r="BK9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BL9" s="72"/>
-      <c r="BM9" s="72" t="s">
+      <c r="BL9" s="78"/>
+      <c r="BM9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BN9" s="72"/>
-      <c r="BO9" s="72" t="s">
+      <c r="BN9" s="78"/>
+      <c r="BO9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BP9" s="72"/>
-      <c r="BQ9" s="72" t="s">
+      <c r="BP9" s="78"/>
+      <c r="BQ9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BR9" s="72"/>
-      <c r="BS9" s="72" t="s">
+      <c r="BR9" s="78"/>
+      <c r="BS9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BT9" s="72"/>
-      <c r="BU9" s="72" t="s">
+      <c r="BT9" s="78"/>
+      <c r="BU9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="BV9" s="72"/>
-      <c r="BW9" s="72"/>
+      <c r="BV9" s="78"/>
+      <c r="BW9" s="78"/>
     </row>
     <row r="10" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="79"/>
       <c r="B10" s="79"/>
-      <c r="C10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="E10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="F10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="G10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="H10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="I10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="J10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="K10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="L10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="M10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="N10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="O10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="P10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="Q10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="R10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="S10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="T10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="U10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="V10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="W10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="X10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="Y10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="Z10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AA10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AB10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AC10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AD10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AE10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AF10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AG10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AH10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AI10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AJ10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AK10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AL10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AM10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AN10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AO10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AP10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AQ10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AR10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AS10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AT10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AU10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AV10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AW10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AX10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="AY10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="AZ10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BA10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BB10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BC10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BD10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BE10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BF10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BG10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BH10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BI10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BJ10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BK10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BL10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BM10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BN10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BO10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BP10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BQ10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BR10" s="39">
-        <v>2021</v>
-      </c>
-      <c r="BS10" s="39">
-        <v>2020</v>
-      </c>
-      <c r="BT10" s="39">
-        <v>2021</v>
-      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="72"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="72"/>
+      <c r="X10" s="72"/>
+      <c r="Y10" s="72"/>
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="72"/>
+      <c r="AB10" s="72"/>
+      <c r="AC10" s="72"/>
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="72"/>
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="72"/>
+      <c r="AH10" s="72"/>
+      <c r="AI10" s="72"/>
+      <c r="AJ10" s="72"/>
+      <c r="AK10" s="72"/>
+      <c r="AL10" s="72"/>
+      <c r="AM10" s="72"/>
+      <c r="AN10" s="72"/>
+      <c r="AO10" s="72"/>
+      <c r="AP10" s="72"/>
+      <c r="AQ10" s="72"/>
+      <c r="AR10" s="72"/>
+      <c r="AS10" s="72"/>
+      <c r="AT10" s="72"/>
+      <c r="AU10" s="72"/>
+      <c r="AV10" s="72"/>
+      <c r="AW10" s="72"/>
+      <c r="AX10" s="72"/>
+      <c r="AY10" s="72"/>
+      <c r="AZ10" s="72"/>
+      <c r="BA10" s="72"/>
+      <c r="BB10" s="72"/>
+      <c r="BC10" s="72"/>
+      <c r="BD10" s="72"/>
+      <c r="BE10" s="72"/>
+      <c r="BF10" s="72"/>
+      <c r="BG10" s="72"/>
+      <c r="BH10" s="72"/>
+      <c r="BI10" s="72"/>
+      <c r="BJ10" s="72"/>
+      <c r="BK10" s="72"/>
+      <c r="BL10" s="72"/>
+      <c r="BM10" s="72"/>
+      <c r="BN10" s="72"/>
+      <c r="BO10" s="72"/>
+      <c r="BP10" s="72"/>
+      <c r="BQ10" s="72"/>
+      <c r="BR10" s="72"/>
+      <c r="BS10" s="72"/>
+      <c r="BT10" s="72"/>
       <c r="BU10" s="38" t="s">
         <v>3</v>
       </c>
       <c r="BV10" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="BW10" s="72"/>
+      <c r="BW10" s="78"/>
     </row>
     <row r="11" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="37">
@@ -87918,9 +87781,9 @@
       <c r="B415" s="30"/>
       <c r="C415" s="55"/>
       <c r="D415" s="55"/>
-      <c r="E415" s="74"/>
-      <c r="F415" s="74"/>
-      <c r="G415" s="74"/>
+      <c r="E415" s="73"/>
+      <c r="F415" s="73"/>
+      <c r="G415" s="73"/>
     </row>
     <row r="416" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A416" s="30"/>
@@ -88374,39 +88237,38 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="E415:G415"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AU9:AV9"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AI9:AJ9"/>
-    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="BM8:BN8"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="BQ8:BR8"/>
+    <mergeCell ref="BS8:BV8"/>
+    <mergeCell ref="BW8:BW10"/>
+    <mergeCell ref="BS9:BT9"/>
+    <mergeCell ref="BU9:BV9"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="BE8:BF8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BI8:BJ8"/>
+    <mergeCell ref="BK8:BL8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AW8:AX8"/>
+    <mergeCell ref="AY8:AZ8"/>
+    <mergeCell ref="BA8:BB8"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AG8:AH8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
     <mergeCell ref="S8:T8"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="W8:X8"/>
@@ -88423,38 +88285,39 @@
     <mergeCell ref="BE9:BF9"/>
     <mergeCell ref="AM9:AN9"/>
     <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AG8:AH8"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AK8:AL8"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AW8:AX8"/>
-    <mergeCell ref="AY8:AZ8"/>
-    <mergeCell ref="BA8:BB8"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="BE8:BF8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BI8:BJ8"/>
-    <mergeCell ref="BK8:BL8"/>
-    <mergeCell ref="BM8:BN8"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="BQ8:BR8"/>
-    <mergeCell ref="BS8:BV8"/>
-    <mergeCell ref="BW8:BW10"/>
-    <mergeCell ref="BS9:BT9"/>
-    <mergeCell ref="BU9:BV9"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AU9:AV9"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AI9:AJ9"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E415:G415"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.31496062992125984" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Laporan orperasi perpolda done
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_detail_daily.xlsx
+++ b/public/template/excel/format_laporan_detail_daily.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Laphar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="331">
   <si>
     <t>URAIAN</t>
   </si>
@@ -1087,6 +1087,15 @@
   <si>
     <t>Pelabuhan</t>
   </si>
+  <si>
+    <t>MARKAS BESAR</t>
+  </si>
+  <si>
+    <t>KEPOLISIAN NEGARA REPUBLIK INDONESIA</t>
+  </si>
+  <si>
+    <t>KORPS LALU LINTAS</t>
+  </si>
 </sst>
 </file>
 
@@ -1095,7 +1104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1196,6 +1205,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1211,7 +1237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1427,12 +1453,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1569,9 +1604,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1620,29 +1652,44 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1664,237 +1711,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>21694</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104742</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2251627</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>111401</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Connector 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="21694" y="590517"/>
-          <a:ext cx="2506158" cy="6659"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>45140</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2377109</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="45140"/>
-          <a:ext cx="2653334" cy="621610"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>MARKAS</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> BESAR</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>KEPOLISIAN NEGARA REPUBLIK INDONESIA</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>KORPS LALU LINTAS</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>606405</xdr:colOff>
-      <xdr:row>416</xdr:row>
-      <xdr:rowOff>166146</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>68035</xdr:colOff>
-      <xdr:row>425</xdr:row>
-      <xdr:rowOff>133015</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5935869" y="72091235"/>
-          <a:ext cx="2523237" cy="1497673"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="1" baseline="0">
-              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>KA POSKO</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1000" b="1" baseline="0">
-            <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1000" b="1" baseline="0">
-            <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1000" b="1" baseline="0">
-            <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2242,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW465"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:BT10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="AX408" zoomScale="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="BT423" sqref="BT423:BW423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2260,433 +2076,643 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A1" s="75"/>
+      <c r="A1" s="75" t="s">
+        <v>328</v>
+      </c>
       <c r="B1" s="75"/>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
+    <row r="2" spans="1:75" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>329</v>
+      </c>
       <c r="B2" s="75"/>
+      <c r="C2" s="72"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="76"/>
+      <c r="A3" s="77" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="77"/>
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="78"/>
+      <c r="AD5" s="78"/>
+      <c r="AE5" s="78"/>
+      <c r="AF5" s="78"/>
+      <c r="AG5" s="78"/>
+      <c r="AH5" s="78"/>
+      <c r="AI5" s="78"/>
+      <c r="AJ5" s="78"/>
+      <c r="AK5" s="78"/>
+      <c r="AL5" s="78"/>
+      <c r="AM5" s="78"/>
+      <c r="AN5" s="78"/>
+      <c r="AO5" s="78"/>
+      <c r="AP5" s="78"/>
+      <c r="AQ5" s="78"/>
+      <c r="AR5" s="78"/>
+      <c r="AS5" s="78"/>
+      <c r="AT5" s="78"/>
+      <c r="AU5" s="78"/>
+      <c r="AV5" s="78"/>
+      <c r="AW5" s="78"/>
+      <c r="AX5" s="78"/>
+      <c r="AY5" s="78"/>
+      <c r="AZ5" s="78"/>
+      <c r="BA5" s="78"/>
+      <c r="BB5" s="78"/>
+      <c r="BC5" s="78"/>
+      <c r="BD5" s="78"/>
+      <c r="BE5" s="78"/>
+      <c r="BF5" s="78"/>
+      <c r="BG5" s="78"/>
+      <c r="BH5" s="78"/>
+      <c r="BI5" s="78"/>
+      <c r="BJ5" s="78"/>
+      <c r="BK5" s="78"/>
+      <c r="BL5" s="78"/>
+      <c r="BM5" s="78"/>
+      <c r="BN5" s="78"/>
+      <c r="BO5" s="78"/>
+      <c r="BP5" s="78"/>
+      <c r="BQ5" s="78"/>
+      <c r="BR5" s="78"/>
+      <c r="BS5" s="78"/>
+      <c r="BT5" s="78"/>
+      <c r="BU5" s="78"/>
+      <c r="BV5" s="78"/>
+      <c r="BW5" s="78"/>
     </row>
     <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="79" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="79"/>
+      <c r="AD6" s="79"/>
+      <c r="AE6" s="79"/>
+      <c r="AF6" s="79"/>
+      <c r="AG6" s="79"/>
+      <c r="AH6" s="79"/>
+      <c r="AI6" s="79"/>
+      <c r="AJ6" s="79"/>
+      <c r="AK6" s="79"/>
+      <c r="AL6" s="79"/>
+      <c r="AM6" s="79"/>
+      <c r="AN6" s="79"/>
+      <c r="AO6" s="79"/>
+      <c r="AP6" s="79"/>
+      <c r="AQ6" s="79"/>
+      <c r="AR6" s="79"/>
+      <c r="AS6" s="79"/>
+      <c r="AT6" s="79"/>
+      <c r="AU6" s="79"/>
+      <c r="AV6" s="79"/>
+      <c r="AW6" s="79"/>
+      <c r="AX6" s="79"/>
+      <c r="AY6" s="79"/>
+      <c r="AZ6" s="79"/>
+      <c r="BA6" s="79"/>
+      <c r="BB6" s="79"/>
+      <c r="BC6" s="79"/>
+      <c r="BD6" s="79"/>
+      <c r="BE6" s="79"/>
+      <c r="BF6" s="79"/>
+      <c r="BG6" s="79"/>
+      <c r="BH6" s="79"/>
+      <c r="BI6" s="79"/>
+      <c r="BJ6" s="79"/>
+      <c r="BK6" s="79"/>
+      <c r="BL6" s="79"/>
+      <c r="BM6" s="79"/>
+      <c r="BN6" s="79"/>
+      <c r="BO6" s="79"/>
+      <c r="BP6" s="79"/>
+      <c r="BQ6" s="79"/>
+      <c r="BR6" s="79"/>
+      <c r="BS6" s="79"/>
+      <c r="BT6" s="79"/>
+      <c r="BU6" s="79"/>
+      <c r="BV6" s="79"/>
+      <c r="BW6" s="79"/>
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="80" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="56"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="80"/>
+      <c r="AA7" s="80"/>
+      <c r="AB7" s="80"/>
+      <c r="AC7" s="80"/>
+      <c r="AD7" s="80"/>
+      <c r="AE7" s="80"/>
+      <c r="AF7" s="80"/>
+      <c r="AG7" s="80"/>
+      <c r="AH7" s="80"/>
+      <c r="AI7" s="80"/>
+      <c r="AJ7" s="80"/>
+      <c r="AK7" s="80"/>
+      <c r="AL7" s="80"/>
+      <c r="AM7" s="80"/>
+      <c r="AN7" s="80"/>
+      <c r="AO7" s="80"/>
+      <c r="AP7" s="80"/>
+      <c r="AQ7" s="80"/>
+      <c r="AR7" s="80"/>
+      <c r="AS7" s="80"/>
+      <c r="AT7" s="80"/>
+      <c r="AU7" s="80"/>
+      <c r="AV7" s="80"/>
+      <c r="AW7" s="80"/>
+      <c r="AX7" s="80"/>
+      <c r="AY7" s="80"/>
+      <c r="AZ7" s="80"/>
+      <c r="BA7" s="80"/>
+      <c r="BB7" s="80"/>
+      <c r="BC7" s="80"/>
+      <c r="BD7" s="80"/>
+      <c r="BE7" s="80"/>
+      <c r="BF7" s="80"/>
+      <c r="BG7" s="80"/>
+      <c r="BH7" s="80"/>
+      <c r="BI7" s="80"/>
+      <c r="BJ7" s="80"/>
+      <c r="BK7" s="80"/>
+      <c r="BL7" s="80"/>
+      <c r="BM7" s="80"/>
+      <c r="BN7" s="80"/>
+      <c r="BO7" s="80"/>
+      <c r="BP7" s="80"/>
+      <c r="BQ7" s="80"/>
+      <c r="BR7" s="80"/>
+      <c r="BS7" s="80"/>
+      <c r="BT7" s="80"/>
+      <c r="BU7" s="80"/>
+      <c r="BV7" s="80"/>
+      <c r="BW7" s="80"/>
     </row>
     <row r="8" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>326</v>
       </c>
-      <c r="B8" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="78" t="s">
+      <c r="B8" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="73" t="s">
         <v>291</v>
       </c>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="73" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78" t="s">
+      <c r="F8" s="73"/>
+      <c r="G8" s="73" t="s">
         <v>293</v>
       </c>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78" t="s">
+      <c r="H8" s="73"/>
+      <c r="I8" s="73" t="s">
         <v>294</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78" t="s">
+      <c r="J8" s="73"/>
+      <c r="K8" s="73" t="s">
         <v>295</v>
       </c>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78" t="s">
+      <c r="L8" s="73"/>
+      <c r="M8" s="73" t="s">
         <v>296</v>
       </c>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78" t="s">
+      <c r="N8" s="73"/>
+      <c r="O8" s="73" t="s">
         <v>297</v>
       </c>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78" t="s">
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73" t="s">
         <v>298</v>
       </c>
-      <c r="R8" s="78"/>
-      <c r="S8" s="78" t="s">
+      <c r="R8" s="73"/>
+      <c r="S8" s="73" t="s">
         <v>299</v>
       </c>
-      <c r="T8" s="78"/>
-      <c r="U8" s="78" t="s">
+      <c r="T8" s="73"/>
+      <c r="U8" s="73" t="s">
         <v>300</v>
       </c>
-      <c r="V8" s="78"/>
-      <c r="W8" s="78" t="s">
+      <c r="V8" s="73"/>
+      <c r="W8" s="73" t="s">
         <v>301</v>
       </c>
-      <c r="X8" s="78"/>
-      <c r="Y8" s="78" t="s">
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73" t="s">
         <v>302</v>
       </c>
-      <c r="Z8" s="78"/>
-      <c r="AA8" s="78" t="s">
+      <c r="Z8" s="73"/>
+      <c r="AA8" s="73" t="s">
         <v>303</v>
       </c>
-      <c r="AB8" s="78"/>
-      <c r="AC8" s="78" t="s">
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="73" t="s">
         <v>304</v>
       </c>
-      <c r="AD8" s="78"/>
-      <c r="AE8" s="78" t="s">
+      <c r="AD8" s="73"/>
+      <c r="AE8" s="73" t="s">
         <v>305</v>
       </c>
-      <c r="AF8" s="78"/>
-      <c r="AG8" s="78" t="s">
+      <c r="AF8" s="73"/>
+      <c r="AG8" s="73" t="s">
         <v>306</v>
       </c>
-      <c r="AH8" s="78"/>
-      <c r="AI8" s="78" t="s">
+      <c r="AH8" s="73"/>
+      <c r="AI8" s="73" t="s">
         <v>307</v>
       </c>
-      <c r="AJ8" s="78"/>
-      <c r="AK8" s="78" t="s">
+      <c r="AJ8" s="73"/>
+      <c r="AK8" s="73" t="s">
         <v>308</v>
       </c>
-      <c r="AL8" s="78"/>
-      <c r="AM8" s="78" t="s">
+      <c r="AL8" s="73"/>
+      <c r="AM8" s="73" t="s">
         <v>309</v>
       </c>
-      <c r="AN8" s="78"/>
-      <c r="AO8" s="78" t="s">
+      <c r="AN8" s="73"/>
+      <c r="AO8" s="73" t="s">
         <v>310</v>
       </c>
-      <c r="AP8" s="78"/>
-      <c r="AQ8" s="78" t="s">
+      <c r="AP8" s="73"/>
+      <c r="AQ8" s="73" t="s">
         <v>311</v>
       </c>
-      <c r="AR8" s="78"/>
-      <c r="AS8" s="78" t="s">
+      <c r="AR8" s="73"/>
+      <c r="AS8" s="73" t="s">
         <v>312</v>
       </c>
-      <c r="AT8" s="78"/>
-      <c r="AU8" s="78" t="s">
+      <c r="AT8" s="73"/>
+      <c r="AU8" s="73" t="s">
         <v>313</v>
       </c>
-      <c r="AV8" s="78"/>
-      <c r="AW8" s="78" t="s">
+      <c r="AV8" s="73"/>
+      <c r="AW8" s="73" t="s">
         <v>314</v>
       </c>
-      <c r="AX8" s="78"/>
-      <c r="AY8" s="78" t="s">
+      <c r="AX8" s="73"/>
+      <c r="AY8" s="73" t="s">
         <v>315</v>
       </c>
-      <c r="AZ8" s="78"/>
-      <c r="BA8" s="78" t="s">
+      <c r="AZ8" s="73"/>
+      <c r="BA8" s="73" t="s">
         <v>316</v>
       </c>
-      <c r="BB8" s="78"/>
-      <c r="BC8" s="80" t="s">
+      <c r="BB8" s="73"/>
+      <c r="BC8" s="81" t="s">
         <v>317</v>
       </c>
-      <c r="BD8" s="80"/>
-      <c r="BE8" s="78" t="s">
+      <c r="BD8" s="81"/>
+      <c r="BE8" s="73" t="s">
         <v>318</v>
       </c>
-      <c r="BF8" s="78"/>
-      <c r="BG8" s="78" t="s">
+      <c r="BF8" s="73"/>
+      <c r="BG8" s="73" t="s">
         <v>319</v>
       </c>
-      <c r="BH8" s="78"/>
-      <c r="BI8" s="78" t="s">
+      <c r="BH8" s="73"/>
+      <c r="BI8" s="73" t="s">
         <v>320</v>
       </c>
-      <c r="BJ8" s="78"/>
-      <c r="BK8" s="78" t="s">
+      <c r="BJ8" s="73"/>
+      <c r="BK8" s="73" t="s">
         <v>321</v>
       </c>
-      <c r="BL8" s="78"/>
-      <c r="BM8" s="78" t="s">
+      <c r="BL8" s="73"/>
+      <c r="BM8" s="73" t="s">
         <v>322</v>
       </c>
-      <c r="BN8" s="78"/>
-      <c r="BO8" s="78" t="s">
+      <c r="BN8" s="73"/>
+      <c r="BO8" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="BP8" s="78"/>
-      <c r="BQ8" s="78" t="s">
+      <c r="BP8" s="73"/>
+      <c r="BQ8" s="73" t="s">
         <v>324</v>
       </c>
-      <c r="BR8" s="78"/>
-      <c r="BS8" s="78" t="s">
+      <c r="BR8" s="73"/>
+      <c r="BS8" s="73" t="s">
         <v>325</v>
       </c>
-      <c r="BT8" s="78"/>
-      <c r="BU8" s="78"/>
-      <c r="BV8" s="78"/>
-      <c r="BW8" s="78" t="s">
+      <c r="BT8" s="73"/>
+      <c r="BU8" s="73"/>
+      <c r="BV8" s="73"/>
+      <c r="BW8" s="73" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="78" t="s">
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78" t="s">
+      <c r="D9" s="73"/>
+      <c r="E9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78" t="s">
+      <c r="F9" s="73"/>
+      <c r="G9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78" t="s">
+      <c r="J9" s="73"/>
+      <c r="K9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78" t="s">
+      <c r="L9" s="73"/>
+      <c r="M9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78" t="s">
+      <c r="N9" s="73"/>
+      <c r="O9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78" t="s">
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78" t="s">
+      <c r="R9" s="73"/>
+      <c r="S9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78" t="s">
+      <c r="T9" s="73"/>
+      <c r="U9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78" t="s">
+      <c r="V9" s="73"/>
+      <c r="W9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="X9" s="78"/>
-      <c r="Y9" s="78" t="s">
+      <c r="X9" s="73"/>
+      <c r="Y9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78" t="s">
+      <c r="Z9" s="73"/>
+      <c r="AA9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AB9" s="78"/>
-      <c r="AC9" s="78" t="s">
+      <c r="AB9" s="73"/>
+      <c r="AC9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AD9" s="78"/>
-      <c r="AE9" s="78" t="s">
+      <c r="AD9" s="73"/>
+      <c r="AE9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="78" t="s">
+      <c r="AF9" s="73"/>
+      <c r="AG9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AH9" s="78"/>
-      <c r="AI9" s="78" t="s">
+      <c r="AH9" s="73"/>
+      <c r="AI9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AJ9" s="78"/>
-      <c r="AK9" s="78" t="s">
+      <c r="AJ9" s="73"/>
+      <c r="AK9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AL9" s="78"/>
-      <c r="AM9" s="78" t="s">
+      <c r="AL9" s="73"/>
+      <c r="AM9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AN9" s="78"/>
-      <c r="AO9" s="78" t="s">
+      <c r="AN9" s="73"/>
+      <c r="AO9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AP9" s="78"/>
-      <c r="AQ9" s="78" t="s">
+      <c r="AP9" s="73"/>
+      <c r="AQ9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AR9" s="78"/>
-      <c r="AS9" s="78" t="s">
+      <c r="AR9" s="73"/>
+      <c r="AS9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AT9" s="78"/>
-      <c r="AU9" s="78" t="s">
+      <c r="AT9" s="73"/>
+      <c r="AU9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AV9" s="78"/>
-      <c r="AW9" s="78" t="s">
+      <c r="AV9" s="73"/>
+      <c r="AW9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AX9" s="78"/>
-      <c r="AY9" s="78" t="s">
+      <c r="AX9" s="73"/>
+      <c r="AY9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="AZ9" s="78"/>
-      <c r="BA9" s="78" t="s">
+      <c r="AZ9" s="73"/>
+      <c r="BA9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BB9" s="78"/>
-      <c r="BC9" s="80" t="s">
+      <c r="BB9" s="73"/>
+      <c r="BC9" s="81" t="s">
         <v>168</v>
       </c>
-      <c r="BD9" s="80"/>
-      <c r="BE9" s="78" t="s">
+      <c r="BD9" s="81"/>
+      <c r="BE9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BF9" s="78"/>
-      <c r="BG9" s="78" t="s">
+      <c r="BF9" s="73"/>
+      <c r="BG9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BH9" s="78"/>
-      <c r="BI9" s="78" t="s">
+      <c r="BH9" s="73"/>
+      <c r="BI9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BJ9" s="78"/>
-      <c r="BK9" s="78" t="s">
+      <c r="BJ9" s="73"/>
+      <c r="BK9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BL9" s="78"/>
-      <c r="BM9" s="78" t="s">
+      <c r="BL9" s="73"/>
+      <c r="BM9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BN9" s="78"/>
-      <c r="BO9" s="78" t="s">
+      <c r="BN9" s="73"/>
+      <c r="BO9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BP9" s="78"/>
-      <c r="BQ9" s="78" t="s">
+      <c r="BP9" s="73"/>
+      <c r="BQ9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BR9" s="78"/>
-      <c r="BS9" s="78" t="s">
+      <c r="BR9" s="73"/>
+      <c r="BS9" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="BT9" s="78"/>
-      <c r="BU9" s="78" t="s">
+      <c r="BT9" s="73"/>
+      <c r="BU9" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="BV9" s="78"/>
-      <c r="BW9" s="78"/>
+      <c r="BV9" s="73"/>
+      <c r="BW9" s="73"/>
     </row>
     <row r="10" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="72"/>
-      <c r="U10" s="72"/>
-      <c r="V10" s="72"/>
-      <c r="W10" s="72"/>
-      <c r="X10" s="72"/>
-      <c r="Y10" s="72"/>
-      <c r="Z10" s="72"/>
-      <c r="AA10" s="72"/>
-      <c r="AB10" s="72"/>
-      <c r="AC10" s="72"/>
-      <c r="AD10" s="72"/>
-      <c r="AE10" s="72"/>
-      <c r="AF10" s="72"/>
-      <c r="AG10" s="72"/>
-      <c r="AH10" s="72"/>
-      <c r="AI10" s="72"/>
-      <c r="AJ10" s="72"/>
-      <c r="AK10" s="72"/>
-      <c r="AL10" s="72"/>
-      <c r="AM10" s="72"/>
-      <c r="AN10" s="72"/>
-      <c r="AO10" s="72"/>
-      <c r="AP10" s="72"/>
-      <c r="AQ10" s="72"/>
-      <c r="AR10" s="72"/>
-      <c r="AS10" s="72"/>
-      <c r="AT10" s="72"/>
-      <c r="AU10" s="72"/>
-      <c r="AV10" s="72"/>
-      <c r="AW10" s="72"/>
-      <c r="AX10" s="72"/>
-      <c r="AY10" s="72"/>
-      <c r="AZ10" s="72"/>
-      <c r="BA10" s="72"/>
-      <c r="BB10" s="72"/>
-      <c r="BC10" s="72"/>
-      <c r="BD10" s="72"/>
-      <c r="BE10" s="72"/>
-      <c r="BF10" s="72"/>
-      <c r="BG10" s="72"/>
-      <c r="BH10" s="72"/>
-      <c r="BI10" s="72"/>
-      <c r="BJ10" s="72"/>
-      <c r="BK10" s="72"/>
-      <c r="BL10" s="72"/>
-      <c r="BM10" s="72"/>
-      <c r="BN10" s="72"/>
-      <c r="BO10" s="72"/>
-      <c r="BP10" s="72"/>
-      <c r="BQ10" s="72"/>
-      <c r="BR10" s="72"/>
-      <c r="BS10" s="72"/>
-      <c r="BT10" s="72"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="71"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="71"/>
+      <c r="AA10" s="71"/>
+      <c r="AB10" s="71"/>
+      <c r="AC10" s="71"/>
+      <c r="AD10" s="71"/>
+      <c r="AE10" s="71"/>
+      <c r="AF10" s="71"/>
+      <c r="AG10" s="71"/>
+      <c r="AH10" s="71"/>
+      <c r="AI10" s="71"/>
+      <c r="AJ10" s="71"/>
+      <c r="AK10" s="71"/>
+      <c r="AL10" s="71"/>
+      <c r="AM10" s="71"/>
+      <c r="AN10" s="71"/>
+      <c r="AO10" s="71"/>
+      <c r="AP10" s="71"/>
+      <c r="AQ10" s="71"/>
+      <c r="AR10" s="71"/>
+      <c r="AS10" s="71"/>
+      <c r="AT10" s="71"/>
+      <c r="AU10" s="71"/>
+      <c r="AV10" s="71"/>
+      <c r="AW10" s="71"/>
+      <c r="AX10" s="71"/>
+      <c r="AY10" s="71"/>
+      <c r="AZ10" s="71"/>
+      <c r="BA10" s="71"/>
+      <c r="BB10" s="71"/>
+      <c r="BC10" s="71"/>
+      <c r="BD10" s="71"/>
+      <c r="BE10" s="71"/>
+      <c r="BF10" s="71"/>
+      <c r="BG10" s="71"/>
+      <c r="BH10" s="71"/>
+      <c r="BI10" s="71"/>
+      <c r="BJ10" s="71"/>
+      <c r="BK10" s="71"/>
+      <c r="BL10" s="71"/>
+      <c r="BM10" s="71"/>
+      <c r="BN10" s="71"/>
+      <c r="BO10" s="71"/>
+      <c r="BP10" s="71"/>
+      <c r="BQ10" s="71"/>
+      <c r="BR10" s="71"/>
+      <c r="BS10" s="71"/>
+      <c r="BT10" s="71"/>
       <c r="BU10" s="38" t="s">
         <v>3</v>
       </c>
       <c r="BV10" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="BW10" s="78"/>
+      <c r="BW10" s="73"/>
     </row>
     <row r="11" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="37">
@@ -2695,223 +2721,223 @@
       <c r="B11" s="37">
         <v>2</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="56">
         <v>1</v>
       </c>
-      <c r="D11" s="57">
+      <c r="D11" s="56">
         <v>2</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="56">
         <v>3</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="56">
         <v>4</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="56">
         <v>5</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="56">
         <v>6</v>
       </c>
-      <c r="I11" s="57">
+      <c r="I11" s="56">
         <v>7</v>
       </c>
-      <c r="J11" s="57">
+      <c r="J11" s="56">
         <v>8</v>
       </c>
-      <c r="K11" s="57">
+      <c r="K11" s="56">
         <v>9</v>
       </c>
-      <c r="L11" s="57">
+      <c r="L11" s="56">
         <v>10</v>
       </c>
-      <c r="M11" s="57">
+      <c r="M11" s="56">
         <v>11</v>
       </c>
-      <c r="N11" s="57">
+      <c r="N11" s="56">
         <v>12</v>
       </c>
-      <c r="O11" s="57">
+      <c r="O11" s="56">
         <v>13</v>
       </c>
-      <c r="P11" s="57">
+      <c r="P11" s="56">
         <v>14</v>
       </c>
-      <c r="Q11" s="57">
+      <c r="Q11" s="56">
         <v>15</v>
       </c>
-      <c r="R11" s="57">
+      <c r="R11" s="56">
         <v>16</v>
       </c>
-      <c r="S11" s="57">
+      <c r="S11" s="56">
         <v>17</v>
       </c>
-      <c r="T11" s="57">
+      <c r="T11" s="56">
         <v>18</v>
       </c>
-      <c r="U11" s="57">
+      <c r="U11" s="56">
         <v>19</v>
       </c>
-      <c r="V11" s="57">
+      <c r="V11" s="56">
         <v>20</v>
       </c>
-      <c r="W11" s="57">
+      <c r="W11" s="56">
         <v>21</v>
       </c>
-      <c r="X11" s="57">
+      <c r="X11" s="56">
         <v>22</v>
       </c>
-      <c r="Y11" s="57">
+      <c r="Y11" s="56">
         <v>23</v>
       </c>
-      <c r="Z11" s="57">
+      <c r="Z11" s="56">
         <v>24</v>
       </c>
-      <c r="AA11" s="57">
+      <c r="AA11" s="56">
         <v>25</v>
       </c>
-      <c r="AB11" s="57">
+      <c r="AB11" s="56">
         <v>26</v>
       </c>
-      <c r="AC11" s="57">
+      <c r="AC11" s="56">
         <v>27</v>
       </c>
-      <c r="AD11" s="57">
+      <c r="AD11" s="56">
         <v>28</v>
       </c>
-      <c r="AE11" s="57">
+      <c r="AE11" s="56">
         <v>29</v>
       </c>
-      <c r="AF11" s="57">
+      <c r="AF11" s="56">
         <v>30</v>
       </c>
-      <c r="AG11" s="57">
+      <c r="AG11" s="56">
         <v>31</v>
       </c>
-      <c r="AH11" s="57">
+      <c r="AH11" s="56">
         <v>32</v>
       </c>
-      <c r="AI11" s="57">
+      <c r="AI11" s="56">
         <v>33</v>
       </c>
-      <c r="AJ11" s="57">
+      <c r="AJ11" s="56">
         <v>34</v>
       </c>
-      <c r="AK11" s="57">
+      <c r="AK11" s="56">
         <v>35</v>
       </c>
-      <c r="AL11" s="57">
+      <c r="AL11" s="56">
         <v>36</v>
       </c>
-      <c r="AM11" s="57">
+      <c r="AM11" s="56">
         <v>37</v>
       </c>
-      <c r="AN11" s="57">
+      <c r="AN11" s="56">
         <v>38</v>
       </c>
-      <c r="AO11" s="57">
+      <c r="AO11" s="56">
         <v>39</v>
       </c>
-      <c r="AP11" s="57">
+      <c r="AP11" s="56">
         <v>40</v>
       </c>
-      <c r="AQ11" s="57">
+      <c r="AQ11" s="56">
         <v>41</v>
       </c>
-      <c r="AR11" s="57">
+      <c r="AR11" s="56">
         <v>42</v>
       </c>
-      <c r="AS11" s="57">
+      <c r="AS11" s="56">
         <v>43</v>
       </c>
-      <c r="AT11" s="57">
+      <c r="AT11" s="56">
         <v>44</v>
       </c>
-      <c r="AU11" s="57">
+      <c r="AU11" s="56">
         <v>45</v>
       </c>
-      <c r="AV11" s="57">
+      <c r="AV11" s="56">
         <v>46</v>
       </c>
-      <c r="AW11" s="57">
+      <c r="AW11" s="56">
         <v>47</v>
       </c>
-      <c r="AX11" s="57">
+      <c r="AX11" s="56">
         <v>48</v>
       </c>
-      <c r="AY11" s="57">
+      <c r="AY11" s="56">
         <v>49</v>
       </c>
-      <c r="AZ11" s="57">
+      <c r="AZ11" s="56">
         <v>50</v>
       </c>
-      <c r="BA11" s="57">
+      <c r="BA11" s="56">
         <v>51</v>
       </c>
-      <c r="BB11" s="57">
+      <c r="BB11" s="56">
         <v>52</v>
       </c>
-      <c r="BC11" s="57">
+      <c r="BC11" s="56">
         <v>53</v>
       </c>
-      <c r="BD11" s="57">
+      <c r="BD11" s="56">
         <v>54</v>
       </c>
-      <c r="BE11" s="57">
+      <c r="BE11" s="56">
         <v>55</v>
       </c>
-      <c r="BF11" s="57">
+      <c r="BF11" s="56">
         <v>56</v>
       </c>
-      <c r="BG11" s="57">
+      <c r="BG11" s="56">
         <v>57</v>
       </c>
-      <c r="BH11" s="57">
+      <c r="BH11" s="56">
         <v>58</v>
       </c>
-      <c r="BI11" s="57">
+      <c r="BI11" s="56">
         <v>59</v>
       </c>
-      <c r="BJ11" s="57">
+      <c r="BJ11" s="56">
         <v>60</v>
       </c>
-      <c r="BK11" s="57">
+      <c r="BK11" s="56">
         <v>61</v>
       </c>
-      <c r="BL11" s="57">
+      <c r="BL11" s="56">
         <v>62</v>
       </c>
-      <c r="BM11" s="57">
+      <c r="BM11" s="56">
         <v>63</v>
       </c>
-      <c r="BN11" s="57">
+      <c r="BN11" s="56">
         <v>64</v>
       </c>
-      <c r="BO11" s="57">
+      <c r="BO11" s="56">
         <v>65</v>
       </c>
-      <c r="BP11" s="57">
+      <c r="BP11" s="56">
         <v>66</v>
       </c>
-      <c r="BQ11" s="57">
+      <c r="BQ11" s="56">
         <v>67</v>
       </c>
-      <c r="BR11" s="57">
+      <c r="BR11" s="56">
         <v>68</v>
       </c>
-      <c r="BS11" s="57">
+      <c r="BS11" s="56">
         <v>69</v>
       </c>
-      <c r="BT11" s="57">
+      <c r="BT11" s="56">
         <v>70</v>
       </c>
-      <c r="BU11" s="57">
+      <c r="BU11" s="56">
         <v>71</v>
       </c>
-      <c r="BV11" s="57">
+      <c r="BV11" s="56">
         <v>72</v>
       </c>
-      <c r="BW11" s="57">
+      <c r="BW11" s="56">
         <v>73</v>
       </c>
     </row>
@@ -71349,73 +71375,73 @@
       <c r="B335" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="C335" s="58"/>
+      <c r="C335" s="57"/>
       <c r="D335" s="46"/>
-      <c r="E335" s="58"/>
+      <c r="E335" s="57"/>
       <c r="F335" s="46"/>
-      <c r="G335" s="58"/>
+      <c r="G335" s="57"/>
       <c r="H335" s="46"/>
-      <c r="I335" s="58"/>
+      <c r="I335" s="57"/>
       <c r="J335" s="46"/>
-      <c r="K335" s="58"/>
+      <c r="K335" s="57"/>
       <c r="L335" s="46"/>
-      <c r="M335" s="58"/>
+      <c r="M335" s="57"/>
       <c r="N335" s="46"/>
-      <c r="O335" s="58"/>
+      <c r="O335" s="57"/>
       <c r="P335" s="46"/>
-      <c r="Q335" s="58"/>
+      <c r="Q335" s="57"/>
       <c r="R335" s="46"/>
-      <c r="S335" s="58"/>
+      <c r="S335" s="57"/>
       <c r="T335" s="46"/>
-      <c r="U335" s="58"/>
+      <c r="U335" s="57"/>
       <c r="V335" s="46"/>
-      <c r="W335" s="58"/>
+      <c r="W335" s="57"/>
       <c r="X335" s="46"/>
-      <c r="Y335" s="58"/>
+      <c r="Y335" s="57"/>
       <c r="Z335" s="46"/>
-      <c r="AA335" s="58"/>
+      <c r="AA335" s="57"/>
       <c r="AB335" s="46"/>
-      <c r="AC335" s="58"/>
+      <c r="AC335" s="57"/>
       <c r="AD335" s="46"/>
-      <c r="AE335" s="58"/>
+      <c r="AE335" s="57"/>
       <c r="AF335" s="46"/>
-      <c r="AG335" s="58"/>
+      <c r="AG335" s="57"/>
       <c r="AH335" s="46"/>
-      <c r="AI335" s="58"/>
+      <c r="AI335" s="57"/>
       <c r="AJ335" s="46"/>
-      <c r="AK335" s="58"/>
+      <c r="AK335" s="57"/>
       <c r="AL335" s="46"/>
-      <c r="AM335" s="58"/>
+      <c r="AM335" s="57"/>
       <c r="AN335" s="46"/>
-      <c r="AO335" s="58"/>
+      <c r="AO335" s="57"/>
       <c r="AP335" s="46"/>
-      <c r="AQ335" s="58"/>
+      <c r="AQ335" s="57"/>
       <c r="AR335" s="46"/>
-      <c r="AS335" s="58"/>
+      <c r="AS335" s="57"/>
       <c r="AT335" s="46"/>
-      <c r="AU335" s="58"/>
+      <c r="AU335" s="57"/>
       <c r="AV335" s="46"/>
-      <c r="AW335" s="58"/>
+      <c r="AW335" s="57"/>
       <c r="AX335" s="46"/>
-      <c r="AY335" s="58"/>
+      <c r="AY335" s="57"/>
       <c r="AZ335" s="46"/>
-      <c r="BA335" s="58"/>
+      <c r="BA335" s="57"/>
       <c r="BB335" s="46"/>
-      <c r="BC335" s="58"/>
+      <c r="BC335" s="57"/>
       <c r="BD335" s="46"/>
-      <c r="BE335" s="58"/>
+      <c r="BE335" s="57"/>
       <c r="BF335" s="46"/>
-      <c r="BG335" s="58"/>
+      <c r="BG335" s="57"/>
       <c r="BH335" s="46"/>
-      <c r="BI335" s="58"/>
+      <c r="BI335" s="57"/>
       <c r="BJ335" s="46"/>
-      <c r="BK335" s="58"/>
+      <c r="BK335" s="57"/>
       <c r="BL335" s="46"/>
-      <c r="BM335" s="58"/>
+      <c r="BM335" s="57"/>
       <c r="BN335" s="46"/>
-      <c r="BO335" s="58"/>
+      <c r="BO335" s="57"/>
       <c r="BP335" s="46"/>
-      <c r="BQ335" s="58"/>
+      <c r="BQ335" s="57"/>
       <c r="BR335" s="46"/>
       <c r="BS335" s="42">
         <f t="shared" ref="BS335:BS398" si="20">C335+E335+G335+I335+K335+M335+O335+Q335+S335+U335+W335+Y335+AA335+AC335+AE335+AG335+AI335+AK335+AM335+AO335+AQ335+AS335+AU335+AW335+AY335+BA335+BC335+BE335+BG335+BI335+BK335+BM335+BO335+BQ335</f>
@@ -71437,73 +71463,73 @@
       <c r="B336" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C336" s="59"/>
+      <c r="C336" s="58"/>
       <c r="D336" s="46"/>
-      <c r="E336" s="59"/>
+      <c r="E336" s="58"/>
       <c r="F336" s="46"/>
-      <c r="G336" s="59"/>
+      <c r="G336" s="58"/>
       <c r="H336" s="46"/>
-      <c r="I336" s="59"/>
+      <c r="I336" s="58"/>
       <c r="J336" s="46"/>
-      <c r="K336" s="59"/>
+      <c r="K336" s="58"/>
       <c r="L336" s="46"/>
-      <c r="M336" s="59"/>
+      <c r="M336" s="58"/>
       <c r="N336" s="46"/>
-      <c r="O336" s="59"/>
+      <c r="O336" s="58"/>
       <c r="P336" s="46"/>
-      <c r="Q336" s="59"/>
+      <c r="Q336" s="58"/>
       <c r="R336" s="46"/>
-      <c r="S336" s="59"/>
+      <c r="S336" s="58"/>
       <c r="T336" s="46"/>
-      <c r="U336" s="59"/>
+      <c r="U336" s="58"/>
       <c r="V336" s="46"/>
-      <c r="W336" s="59"/>
+      <c r="W336" s="58"/>
       <c r="X336" s="46"/>
-      <c r="Y336" s="59"/>
+      <c r="Y336" s="58"/>
       <c r="Z336" s="46"/>
-      <c r="AA336" s="59"/>
+      <c r="AA336" s="58"/>
       <c r="AB336" s="46"/>
-      <c r="AC336" s="59"/>
+      <c r="AC336" s="58"/>
       <c r="AD336" s="46"/>
-      <c r="AE336" s="59"/>
+      <c r="AE336" s="58"/>
       <c r="AF336" s="46"/>
-      <c r="AG336" s="59"/>
+      <c r="AG336" s="58"/>
       <c r="AH336" s="46"/>
-      <c r="AI336" s="59"/>
+      <c r="AI336" s="58"/>
       <c r="AJ336" s="46"/>
-      <c r="AK336" s="59"/>
+      <c r="AK336" s="58"/>
       <c r="AL336" s="46"/>
-      <c r="AM336" s="59"/>
+      <c r="AM336" s="58"/>
       <c r="AN336" s="46"/>
-      <c r="AO336" s="59"/>
+      <c r="AO336" s="58"/>
       <c r="AP336" s="46"/>
-      <c r="AQ336" s="59"/>
+      <c r="AQ336" s="58"/>
       <c r="AR336" s="46"/>
-      <c r="AS336" s="59"/>
+      <c r="AS336" s="58"/>
       <c r="AT336" s="46"/>
-      <c r="AU336" s="59"/>
+      <c r="AU336" s="58"/>
       <c r="AV336" s="46"/>
-      <c r="AW336" s="59"/>
+      <c r="AW336" s="58"/>
       <c r="AX336" s="46"/>
-      <c r="AY336" s="59"/>
+      <c r="AY336" s="58"/>
       <c r="AZ336" s="46"/>
-      <c r="BA336" s="59"/>
+      <c r="BA336" s="58"/>
       <c r="BB336" s="46"/>
-      <c r="BC336" s="59"/>
+      <c r="BC336" s="58"/>
       <c r="BD336" s="46"/>
-      <c r="BE336" s="59"/>
+      <c r="BE336" s="58"/>
       <c r="BF336" s="46"/>
-      <c r="BG336" s="59"/>
+      <c r="BG336" s="58"/>
       <c r="BH336" s="46"/>
-      <c r="BI336" s="59"/>
+      <c r="BI336" s="58"/>
       <c r="BJ336" s="46"/>
-      <c r="BK336" s="59"/>
+      <c r="BK336" s="58"/>
       <c r="BL336" s="46"/>
-      <c r="BM336" s="59"/>
+      <c r="BM336" s="58"/>
       <c r="BN336" s="46"/>
-      <c r="BO336" s="59"/>
+      <c r="BO336" s="58"/>
       <c r="BP336" s="46"/>
-      <c r="BQ336" s="59"/>
+      <c r="BQ336" s="58"/>
       <c r="BR336" s="46"/>
       <c r="BS336" s="42">
         <f t="shared" si="20"/>
@@ -73128,73 +73154,73 @@
       <c r="B344" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C344" s="59"/>
+      <c r="C344" s="58"/>
       <c r="D344" s="46"/>
-      <c r="E344" s="59"/>
+      <c r="E344" s="58"/>
       <c r="F344" s="46"/>
-      <c r="G344" s="59"/>
+      <c r="G344" s="58"/>
       <c r="H344" s="46"/>
-      <c r="I344" s="59"/>
+      <c r="I344" s="58"/>
       <c r="J344" s="46"/>
-      <c r="K344" s="59"/>
+      <c r="K344" s="58"/>
       <c r="L344" s="46"/>
-      <c r="M344" s="59"/>
+      <c r="M344" s="58"/>
       <c r="N344" s="46"/>
-      <c r="O344" s="59"/>
+      <c r="O344" s="58"/>
       <c r="P344" s="46"/>
-      <c r="Q344" s="59"/>
+      <c r="Q344" s="58"/>
       <c r="R344" s="46"/>
-      <c r="S344" s="59"/>
+      <c r="S344" s="58"/>
       <c r="T344" s="46"/>
-      <c r="U344" s="59"/>
+      <c r="U344" s="58"/>
       <c r="V344" s="46"/>
-      <c r="W344" s="59"/>
+      <c r="W344" s="58"/>
       <c r="X344" s="46"/>
-      <c r="Y344" s="59"/>
+      <c r="Y344" s="58"/>
       <c r="Z344" s="46"/>
-      <c r="AA344" s="59"/>
+      <c r="AA344" s="58"/>
       <c r="AB344" s="46"/>
-      <c r="AC344" s="59"/>
+      <c r="AC344" s="58"/>
       <c r="AD344" s="46"/>
-      <c r="AE344" s="59"/>
+      <c r="AE344" s="58"/>
       <c r="AF344" s="46"/>
-      <c r="AG344" s="59"/>
+      <c r="AG344" s="58"/>
       <c r="AH344" s="46"/>
-      <c r="AI344" s="59"/>
+      <c r="AI344" s="58"/>
       <c r="AJ344" s="46"/>
-      <c r="AK344" s="59"/>
+      <c r="AK344" s="58"/>
       <c r="AL344" s="46"/>
-      <c r="AM344" s="59"/>
+      <c r="AM344" s="58"/>
       <c r="AN344" s="46"/>
-      <c r="AO344" s="59"/>
+      <c r="AO344" s="58"/>
       <c r="AP344" s="46"/>
-      <c r="AQ344" s="59"/>
+      <c r="AQ344" s="58"/>
       <c r="AR344" s="46"/>
-      <c r="AS344" s="59"/>
+      <c r="AS344" s="58"/>
       <c r="AT344" s="46"/>
-      <c r="AU344" s="59"/>
+      <c r="AU344" s="58"/>
       <c r="AV344" s="46"/>
-      <c r="AW344" s="59"/>
+      <c r="AW344" s="58"/>
       <c r="AX344" s="46"/>
-      <c r="AY344" s="59"/>
+      <c r="AY344" s="58"/>
       <c r="AZ344" s="46"/>
-      <c r="BA344" s="59"/>
+      <c r="BA344" s="58"/>
       <c r="BB344" s="46"/>
-      <c r="BC344" s="59"/>
+      <c r="BC344" s="58"/>
       <c r="BD344" s="46"/>
-      <c r="BE344" s="59"/>
+      <c r="BE344" s="58"/>
       <c r="BF344" s="46"/>
-      <c r="BG344" s="59"/>
+      <c r="BG344" s="58"/>
       <c r="BH344" s="46"/>
-      <c r="BI344" s="59"/>
+      <c r="BI344" s="58"/>
       <c r="BJ344" s="46"/>
-      <c r="BK344" s="59"/>
+      <c r="BK344" s="58"/>
       <c r="BL344" s="46"/>
-      <c r="BM344" s="59"/>
+      <c r="BM344" s="58"/>
       <c r="BN344" s="46"/>
-      <c r="BO344" s="59"/>
+      <c r="BO344" s="58"/>
       <c r="BP344" s="46"/>
-      <c r="BQ344" s="59"/>
+      <c r="BQ344" s="58"/>
       <c r="BR344" s="46"/>
       <c r="BS344" s="42">
         <f t="shared" si="20"/>
@@ -75594,73 +75620,73 @@
       <c r="B356" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="C356" s="59"/>
+      <c r="C356" s="58"/>
       <c r="D356" s="46"/>
-      <c r="E356" s="59"/>
+      <c r="E356" s="58"/>
       <c r="F356" s="46"/>
-      <c r="G356" s="59"/>
+      <c r="G356" s="58"/>
       <c r="H356" s="46"/>
-      <c r="I356" s="59"/>
+      <c r="I356" s="58"/>
       <c r="J356" s="46"/>
-      <c r="K356" s="59"/>
+      <c r="K356" s="58"/>
       <c r="L356" s="46"/>
-      <c r="M356" s="59"/>
+      <c r="M356" s="58"/>
       <c r="N356" s="46"/>
-      <c r="O356" s="59"/>
+      <c r="O356" s="58"/>
       <c r="P356" s="46"/>
-      <c r="Q356" s="59"/>
+      <c r="Q356" s="58"/>
       <c r="R356" s="46"/>
-      <c r="S356" s="59"/>
+      <c r="S356" s="58"/>
       <c r="T356" s="46"/>
-      <c r="U356" s="59"/>
+      <c r="U356" s="58"/>
       <c r="V356" s="46"/>
-      <c r="W356" s="59"/>
+      <c r="W356" s="58"/>
       <c r="X356" s="46"/>
-      <c r="Y356" s="59"/>
+      <c r="Y356" s="58"/>
       <c r="Z356" s="46"/>
-      <c r="AA356" s="59"/>
+      <c r="AA356" s="58"/>
       <c r="AB356" s="46"/>
-      <c r="AC356" s="59"/>
+      <c r="AC356" s="58"/>
       <c r="AD356" s="46"/>
-      <c r="AE356" s="59"/>
+      <c r="AE356" s="58"/>
       <c r="AF356" s="46"/>
-      <c r="AG356" s="59"/>
+      <c r="AG356" s="58"/>
       <c r="AH356" s="46"/>
-      <c r="AI356" s="59"/>
+      <c r="AI356" s="58"/>
       <c r="AJ356" s="46"/>
-      <c r="AK356" s="59"/>
+      <c r="AK356" s="58"/>
       <c r="AL356" s="46"/>
-      <c r="AM356" s="59"/>
+      <c r="AM356" s="58"/>
       <c r="AN356" s="46"/>
-      <c r="AO356" s="59"/>
+      <c r="AO356" s="58"/>
       <c r="AP356" s="46"/>
-      <c r="AQ356" s="59"/>
+      <c r="AQ356" s="58"/>
       <c r="AR356" s="46"/>
-      <c r="AS356" s="59"/>
+      <c r="AS356" s="58"/>
       <c r="AT356" s="46"/>
-      <c r="AU356" s="59"/>
+      <c r="AU356" s="58"/>
       <c r="AV356" s="46"/>
-      <c r="AW356" s="59"/>
+      <c r="AW356" s="58"/>
       <c r="AX356" s="46"/>
-      <c r="AY356" s="59"/>
+      <c r="AY356" s="58"/>
       <c r="AZ356" s="46"/>
-      <c r="BA356" s="59"/>
+      <c r="BA356" s="58"/>
       <c r="BB356" s="46"/>
-      <c r="BC356" s="59"/>
+      <c r="BC356" s="58"/>
       <c r="BD356" s="46"/>
-      <c r="BE356" s="59"/>
+      <c r="BE356" s="58"/>
       <c r="BF356" s="46"/>
-      <c r="BG356" s="59"/>
+      <c r="BG356" s="58"/>
       <c r="BH356" s="46"/>
-      <c r="BI356" s="59"/>
+      <c r="BI356" s="58"/>
       <c r="BJ356" s="46"/>
-      <c r="BK356" s="59"/>
+      <c r="BK356" s="58"/>
       <c r="BL356" s="46"/>
-      <c r="BM356" s="59"/>
+      <c r="BM356" s="58"/>
       <c r="BN356" s="46"/>
-      <c r="BO356" s="59"/>
+      <c r="BO356" s="58"/>
       <c r="BP356" s="46"/>
-      <c r="BQ356" s="59"/>
+      <c r="BQ356" s="58"/>
       <c r="BR356" s="46"/>
       <c r="BS356" s="42">
         <f t="shared" si="20"/>
@@ -77516,73 +77542,73 @@
       <c r="B365" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C365" s="58"/>
+      <c r="C365" s="57"/>
       <c r="D365" s="46"/>
-      <c r="E365" s="58"/>
+      <c r="E365" s="57"/>
       <c r="F365" s="46"/>
-      <c r="G365" s="58"/>
+      <c r="G365" s="57"/>
       <c r="H365" s="46"/>
-      <c r="I365" s="58"/>
+      <c r="I365" s="57"/>
       <c r="J365" s="46"/>
-      <c r="K365" s="58"/>
+      <c r="K365" s="57"/>
       <c r="L365" s="46"/>
-      <c r="M365" s="58"/>
+      <c r="M365" s="57"/>
       <c r="N365" s="46"/>
-      <c r="O365" s="58"/>
+      <c r="O365" s="57"/>
       <c r="P365" s="46"/>
-      <c r="Q365" s="58"/>
+      <c r="Q365" s="57"/>
       <c r="R365" s="46"/>
-      <c r="S365" s="58"/>
+      <c r="S365" s="57"/>
       <c r="T365" s="46"/>
-      <c r="U365" s="58"/>
+      <c r="U365" s="57"/>
       <c r="V365" s="46"/>
-      <c r="W365" s="58"/>
+      <c r="W365" s="57"/>
       <c r="X365" s="46"/>
-      <c r="Y365" s="58"/>
+      <c r="Y365" s="57"/>
       <c r="Z365" s="46"/>
-      <c r="AA365" s="58"/>
+      <c r="AA365" s="57"/>
       <c r="AB365" s="46"/>
-      <c r="AC365" s="58"/>
+      <c r="AC365" s="57"/>
       <c r="AD365" s="46"/>
-      <c r="AE365" s="58"/>
+      <c r="AE365" s="57"/>
       <c r="AF365" s="46"/>
-      <c r="AG365" s="58"/>
+      <c r="AG365" s="57"/>
       <c r="AH365" s="46"/>
-      <c r="AI365" s="58"/>
+      <c r="AI365" s="57"/>
       <c r="AJ365" s="46"/>
-      <c r="AK365" s="58"/>
+      <c r="AK365" s="57"/>
       <c r="AL365" s="46"/>
-      <c r="AM365" s="58"/>
+      <c r="AM365" s="57"/>
       <c r="AN365" s="46"/>
-      <c r="AO365" s="58"/>
+      <c r="AO365" s="57"/>
       <c r="AP365" s="46"/>
-      <c r="AQ365" s="58"/>
+      <c r="AQ365" s="57"/>
       <c r="AR365" s="46"/>
-      <c r="AS365" s="58"/>
+      <c r="AS365" s="57"/>
       <c r="AT365" s="46"/>
-      <c r="AU365" s="58"/>
+      <c r="AU365" s="57"/>
       <c r="AV365" s="46"/>
-      <c r="AW365" s="58"/>
+      <c r="AW365" s="57"/>
       <c r="AX365" s="46"/>
-      <c r="AY365" s="58"/>
+      <c r="AY365" s="57"/>
       <c r="AZ365" s="46"/>
-      <c r="BA365" s="58"/>
+      <c r="BA365" s="57"/>
       <c r="BB365" s="46"/>
-      <c r="BC365" s="58"/>
+      <c r="BC365" s="57"/>
       <c r="BD365" s="46"/>
-      <c r="BE365" s="58"/>
+      <c r="BE365" s="57"/>
       <c r="BF365" s="46"/>
-      <c r="BG365" s="58"/>
+      <c r="BG365" s="57"/>
       <c r="BH365" s="46"/>
-      <c r="BI365" s="58"/>
+      <c r="BI365" s="57"/>
       <c r="BJ365" s="46"/>
-      <c r="BK365" s="58"/>
+      <c r="BK365" s="57"/>
       <c r="BL365" s="46"/>
-      <c r="BM365" s="58"/>
+      <c r="BM365" s="57"/>
       <c r="BN365" s="46"/>
-      <c r="BO365" s="58"/>
+      <c r="BO365" s="57"/>
       <c r="BP365" s="46"/>
-      <c r="BQ365" s="58"/>
+      <c r="BQ365" s="57"/>
       <c r="BR365" s="46"/>
       <c r="BS365" s="42">
         <f t="shared" si="20"/>
@@ -77597,7 +77623,7 @@
         <v>0</v>
       </c>
       <c r="BV365" s="43"/>
-      <c r="BW365" s="58"/>
+      <c r="BW365" s="57"/>
     </row>
     <row r="366" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A366" s="22">
@@ -77606,139 +77632,139 @@
       <c r="B366" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="C366" s="58"/>
+      <c r="C366" s="57"/>
       <c r="D366" s="42">
         <v>0</v>
       </c>
-      <c r="E366" s="58"/>
+      <c r="E366" s="57"/>
       <c r="F366" s="42">
         <v>0</v>
       </c>
-      <c r="G366" s="58"/>
+      <c r="G366" s="57"/>
       <c r="H366" s="42">
         <v>0</v>
       </c>
-      <c r="I366" s="58"/>
+      <c r="I366" s="57"/>
       <c r="J366" s="42">
         <v>0</v>
       </c>
-      <c r="K366" s="58"/>
+      <c r="K366" s="57"/>
       <c r="L366" s="42">
         <v>0</v>
       </c>
-      <c r="M366" s="58"/>
+      <c r="M366" s="57"/>
       <c r="N366" s="42">
         <v>0</v>
       </c>
-      <c r="O366" s="58"/>
+      <c r="O366" s="57"/>
       <c r="P366" s="42">
         <v>0</v>
       </c>
-      <c r="Q366" s="58"/>
+      <c r="Q366" s="57"/>
       <c r="R366" s="42">
         <v>0</v>
       </c>
-      <c r="S366" s="58"/>
+      <c r="S366" s="57"/>
       <c r="T366" s="42">
         <v>0</v>
       </c>
-      <c r="U366" s="58"/>
+      <c r="U366" s="57"/>
       <c r="V366" s="42">
         <v>0</v>
       </c>
-      <c r="W366" s="58"/>
+      <c r="W366" s="57"/>
       <c r="X366" s="42">
         <v>0</v>
       </c>
-      <c r="Y366" s="58"/>
+      <c r="Y366" s="57"/>
       <c r="Z366" s="42">
         <v>0</v>
       </c>
-      <c r="AA366" s="58"/>
+      <c r="AA366" s="57"/>
       <c r="AB366" s="42">
         <v>0</v>
       </c>
-      <c r="AC366" s="58"/>
+      <c r="AC366" s="57"/>
       <c r="AD366" s="42">
         <v>0</v>
       </c>
-      <c r="AE366" s="58"/>
+      <c r="AE366" s="57"/>
       <c r="AF366" s="42">
         <v>0</v>
       </c>
-      <c r="AG366" s="58"/>
+      <c r="AG366" s="57"/>
       <c r="AH366" s="42">
         <v>0</v>
       </c>
-      <c r="AI366" s="58"/>
+      <c r="AI366" s="57"/>
       <c r="AJ366" s="42">
         <v>0</v>
       </c>
-      <c r="AK366" s="58"/>
+      <c r="AK366" s="57"/>
       <c r="AL366" s="42">
         <v>0</v>
       </c>
-      <c r="AM366" s="58"/>
+      <c r="AM366" s="57"/>
       <c r="AN366" s="42">
         <v>0</v>
       </c>
-      <c r="AO366" s="58"/>
+      <c r="AO366" s="57"/>
       <c r="AP366" s="42">
         <v>0</v>
       </c>
-      <c r="AQ366" s="58"/>
+      <c r="AQ366" s="57"/>
       <c r="AR366" s="42">
         <v>0</v>
       </c>
-      <c r="AS366" s="58"/>
+      <c r="AS366" s="57"/>
       <c r="AT366" s="42">
         <v>0</v>
       </c>
-      <c r="AU366" s="58"/>
+      <c r="AU366" s="57"/>
       <c r="AV366" s="42">
         <v>0</v>
       </c>
-      <c r="AW366" s="58"/>
+      <c r="AW366" s="57"/>
       <c r="AX366" s="42">
         <v>0</v>
       </c>
-      <c r="AY366" s="58"/>
+      <c r="AY366" s="57"/>
       <c r="AZ366" s="42">
         <v>0</v>
       </c>
-      <c r="BA366" s="58"/>
+      <c r="BA366" s="57"/>
       <c r="BB366" s="42">
         <v>0</v>
       </c>
-      <c r="BC366" s="58"/>
+      <c r="BC366" s="57"/>
       <c r="BD366" s="42">
         <v>0</v>
       </c>
-      <c r="BE366" s="58"/>
+      <c r="BE366" s="57"/>
       <c r="BF366" s="42">
         <v>0</v>
       </c>
-      <c r="BG366" s="58"/>
+      <c r="BG366" s="57"/>
       <c r="BH366" s="42">
         <v>0</v>
       </c>
-      <c r="BI366" s="58"/>
+      <c r="BI366" s="57"/>
       <c r="BJ366" s="42">
         <v>0</v>
       </c>
-      <c r="BK366" s="58"/>
+      <c r="BK366" s="57"/>
       <c r="BL366" s="42">
         <v>0</v>
       </c>
-      <c r="BM366" s="58"/>
+      <c r="BM366" s="57"/>
       <c r="BN366" s="42">
         <v>0</v>
       </c>
-      <c r="BO366" s="58"/>
+      <c r="BO366" s="57"/>
       <c r="BP366" s="42">
         <v>0</v>
       </c>
-      <c r="BQ366" s="58"/>
+      <c r="BQ366" s="57"/>
       <c r="BR366" s="42">
         <v>0</v>
       </c>
@@ -78912,73 +78938,73 @@
       <c r="B372" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="C372" s="60"/>
+      <c r="C372" s="59"/>
       <c r="D372" s="46"/>
-      <c r="E372" s="60"/>
+      <c r="E372" s="59"/>
       <c r="F372" s="46"/>
-      <c r="G372" s="60"/>
+      <c r="G372" s="59"/>
       <c r="H372" s="46"/>
-      <c r="I372" s="60"/>
+      <c r="I372" s="59"/>
       <c r="J372" s="46"/>
-      <c r="K372" s="60"/>
+      <c r="K372" s="59"/>
       <c r="L372" s="46"/>
-      <c r="M372" s="60"/>
+      <c r="M372" s="59"/>
       <c r="N372" s="46"/>
-      <c r="O372" s="60"/>
+      <c r="O372" s="59"/>
       <c r="P372" s="46"/>
-      <c r="Q372" s="60"/>
+      <c r="Q372" s="59"/>
       <c r="R372" s="46"/>
-      <c r="S372" s="60"/>
+      <c r="S372" s="59"/>
       <c r="T372" s="46"/>
-      <c r="U372" s="60"/>
+      <c r="U372" s="59"/>
       <c r="V372" s="46"/>
-      <c r="W372" s="60"/>
+      <c r="W372" s="59"/>
       <c r="X372" s="46"/>
-      <c r="Y372" s="60"/>
+      <c r="Y372" s="59"/>
       <c r="Z372" s="46"/>
-      <c r="AA372" s="60"/>
+      <c r="AA372" s="59"/>
       <c r="AB372" s="46"/>
-      <c r="AC372" s="60"/>
+      <c r="AC372" s="59"/>
       <c r="AD372" s="46"/>
-      <c r="AE372" s="60"/>
+      <c r="AE372" s="59"/>
       <c r="AF372" s="46"/>
-      <c r="AG372" s="60"/>
+      <c r="AG372" s="59"/>
       <c r="AH372" s="46"/>
-      <c r="AI372" s="60"/>
+      <c r="AI372" s="59"/>
       <c r="AJ372" s="46"/>
-      <c r="AK372" s="60"/>
+      <c r="AK372" s="59"/>
       <c r="AL372" s="46"/>
-      <c r="AM372" s="60"/>
+      <c r="AM372" s="59"/>
       <c r="AN372" s="46"/>
-      <c r="AO372" s="60"/>
+      <c r="AO372" s="59"/>
       <c r="AP372" s="46"/>
-      <c r="AQ372" s="60"/>
+      <c r="AQ372" s="59"/>
       <c r="AR372" s="46"/>
-      <c r="AS372" s="60"/>
+      <c r="AS372" s="59"/>
       <c r="AT372" s="46"/>
-      <c r="AU372" s="60"/>
+      <c r="AU372" s="59"/>
       <c r="AV372" s="46"/>
-      <c r="AW372" s="60"/>
+      <c r="AW372" s="59"/>
       <c r="AX372" s="46"/>
-      <c r="AY372" s="60"/>
+      <c r="AY372" s="59"/>
       <c r="AZ372" s="46"/>
-      <c r="BA372" s="60"/>
+      <c r="BA372" s="59"/>
       <c r="BB372" s="46"/>
-      <c r="BC372" s="60"/>
+      <c r="BC372" s="59"/>
       <c r="BD372" s="46"/>
-      <c r="BE372" s="60"/>
+      <c r="BE372" s="59"/>
       <c r="BF372" s="46"/>
-      <c r="BG372" s="60"/>
+      <c r="BG372" s="59"/>
       <c r="BH372" s="46"/>
-      <c r="BI372" s="60"/>
+      <c r="BI372" s="59"/>
       <c r="BJ372" s="46"/>
-      <c r="BK372" s="60"/>
+      <c r="BK372" s="59"/>
       <c r="BL372" s="46"/>
-      <c r="BM372" s="60"/>
+      <c r="BM372" s="59"/>
       <c r="BN372" s="46"/>
-      <c r="BO372" s="60"/>
+      <c r="BO372" s="59"/>
       <c r="BP372" s="46"/>
-      <c r="BQ372" s="60"/>
+      <c r="BQ372" s="59"/>
       <c r="BR372" s="46"/>
       <c r="BS372" s="42">
         <f t="shared" si="20"/>
@@ -79002,73 +79028,73 @@
       <c r="B373" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="C373" s="61"/>
+      <c r="C373" s="60"/>
       <c r="D373" s="46"/>
-      <c r="E373" s="61"/>
+      <c r="E373" s="60"/>
       <c r="F373" s="46"/>
-      <c r="G373" s="61"/>
+      <c r="G373" s="60"/>
       <c r="H373" s="46"/>
-      <c r="I373" s="61"/>
+      <c r="I373" s="60"/>
       <c r="J373" s="46"/>
-      <c r="K373" s="61"/>
+      <c r="K373" s="60"/>
       <c r="L373" s="46"/>
-      <c r="M373" s="61"/>
+      <c r="M373" s="60"/>
       <c r="N373" s="46"/>
-      <c r="O373" s="61"/>
+      <c r="O373" s="60"/>
       <c r="P373" s="46"/>
-      <c r="Q373" s="61"/>
+      <c r="Q373" s="60"/>
       <c r="R373" s="46"/>
-      <c r="S373" s="61"/>
+      <c r="S373" s="60"/>
       <c r="T373" s="46"/>
-      <c r="U373" s="61"/>
+      <c r="U373" s="60"/>
       <c r="V373" s="46"/>
-      <c r="W373" s="61"/>
+      <c r="W373" s="60"/>
       <c r="X373" s="46"/>
-      <c r="Y373" s="61"/>
+      <c r="Y373" s="60"/>
       <c r="Z373" s="46"/>
-      <c r="AA373" s="61"/>
+      <c r="AA373" s="60"/>
       <c r="AB373" s="46"/>
-      <c r="AC373" s="61"/>
+      <c r="AC373" s="60"/>
       <c r="AD373" s="46"/>
-      <c r="AE373" s="61"/>
+      <c r="AE373" s="60"/>
       <c r="AF373" s="46"/>
-      <c r="AG373" s="61"/>
+      <c r="AG373" s="60"/>
       <c r="AH373" s="46"/>
-      <c r="AI373" s="61"/>
+      <c r="AI373" s="60"/>
       <c r="AJ373" s="46"/>
-      <c r="AK373" s="61"/>
+      <c r="AK373" s="60"/>
       <c r="AL373" s="46"/>
-      <c r="AM373" s="61"/>
+      <c r="AM373" s="60"/>
       <c r="AN373" s="46"/>
-      <c r="AO373" s="61"/>
+      <c r="AO373" s="60"/>
       <c r="AP373" s="46"/>
-      <c r="AQ373" s="61"/>
+      <c r="AQ373" s="60"/>
       <c r="AR373" s="46"/>
-      <c r="AS373" s="61"/>
+      <c r="AS373" s="60"/>
       <c r="AT373" s="46"/>
-      <c r="AU373" s="61"/>
+      <c r="AU373" s="60"/>
       <c r="AV373" s="46"/>
-      <c r="AW373" s="61"/>
+      <c r="AW373" s="60"/>
       <c r="AX373" s="46"/>
-      <c r="AY373" s="61"/>
+      <c r="AY373" s="60"/>
       <c r="AZ373" s="46"/>
-      <c r="BA373" s="61"/>
+      <c r="BA373" s="60"/>
       <c r="BB373" s="46"/>
-      <c r="BC373" s="61"/>
+      <c r="BC373" s="60"/>
       <c r="BD373" s="46"/>
-      <c r="BE373" s="61"/>
+      <c r="BE373" s="60"/>
       <c r="BF373" s="46"/>
-      <c r="BG373" s="61"/>
+      <c r="BG373" s="60"/>
       <c r="BH373" s="46"/>
-      <c r="BI373" s="61"/>
+      <c r="BI373" s="60"/>
       <c r="BJ373" s="46"/>
-      <c r="BK373" s="61"/>
+      <c r="BK373" s="60"/>
       <c r="BL373" s="46"/>
-      <c r="BM373" s="61"/>
+      <c r="BM373" s="60"/>
       <c r="BN373" s="46"/>
-      <c r="BO373" s="61"/>
+      <c r="BO373" s="60"/>
       <c r="BP373" s="46"/>
-      <c r="BQ373" s="61"/>
+      <c r="BQ373" s="60"/>
       <c r="BR373" s="46"/>
       <c r="BS373" s="42">
         <f t="shared" si="20"/>
@@ -79092,73 +79118,73 @@
       <c r="B374" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="C374" s="62"/>
+      <c r="C374" s="61"/>
       <c r="D374" s="46"/>
-      <c r="E374" s="62"/>
+      <c r="E374" s="61"/>
       <c r="F374" s="46"/>
-      <c r="G374" s="62"/>
+      <c r="G374" s="61"/>
       <c r="H374" s="46"/>
-      <c r="I374" s="62"/>
+      <c r="I374" s="61"/>
       <c r="J374" s="46"/>
-      <c r="K374" s="62"/>
+      <c r="K374" s="61"/>
       <c r="L374" s="46"/>
-      <c r="M374" s="62"/>
+      <c r="M374" s="61"/>
       <c r="N374" s="46"/>
-      <c r="O374" s="62"/>
+      <c r="O374" s="61"/>
       <c r="P374" s="46"/>
-      <c r="Q374" s="62"/>
+      <c r="Q374" s="61"/>
       <c r="R374" s="46"/>
-      <c r="S374" s="62"/>
+      <c r="S374" s="61"/>
       <c r="T374" s="46"/>
-      <c r="U374" s="62"/>
+      <c r="U374" s="61"/>
       <c r="V374" s="46"/>
-      <c r="W374" s="62"/>
+      <c r="W374" s="61"/>
       <c r="X374" s="46"/>
-      <c r="Y374" s="62"/>
+      <c r="Y374" s="61"/>
       <c r="Z374" s="46"/>
-      <c r="AA374" s="62"/>
+      <c r="AA374" s="61"/>
       <c r="AB374" s="46"/>
-      <c r="AC374" s="62"/>
+      <c r="AC374" s="61"/>
       <c r="AD374" s="46"/>
-      <c r="AE374" s="62"/>
+      <c r="AE374" s="61"/>
       <c r="AF374" s="46"/>
-      <c r="AG374" s="62"/>
+      <c r="AG374" s="61"/>
       <c r="AH374" s="46"/>
-      <c r="AI374" s="62"/>
+      <c r="AI374" s="61"/>
       <c r="AJ374" s="46"/>
-      <c r="AK374" s="62"/>
+      <c r="AK374" s="61"/>
       <c r="AL374" s="46"/>
-      <c r="AM374" s="62"/>
+      <c r="AM374" s="61"/>
       <c r="AN374" s="46"/>
-      <c r="AO374" s="62"/>
+      <c r="AO374" s="61"/>
       <c r="AP374" s="46"/>
-      <c r="AQ374" s="62"/>
+      <c r="AQ374" s="61"/>
       <c r="AR374" s="46"/>
-      <c r="AS374" s="62"/>
+      <c r="AS374" s="61"/>
       <c r="AT374" s="46"/>
-      <c r="AU374" s="62"/>
+      <c r="AU374" s="61"/>
       <c r="AV374" s="46"/>
-      <c r="AW374" s="62"/>
+      <c r="AW374" s="61"/>
       <c r="AX374" s="46"/>
-      <c r="AY374" s="62"/>
+      <c r="AY374" s="61"/>
       <c r="AZ374" s="46"/>
-      <c r="BA374" s="62"/>
+      <c r="BA374" s="61"/>
       <c r="BB374" s="46"/>
-      <c r="BC374" s="62"/>
+      <c r="BC374" s="61"/>
       <c r="BD374" s="46"/>
-      <c r="BE374" s="62"/>
+      <c r="BE374" s="61"/>
       <c r="BF374" s="46"/>
-      <c r="BG374" s="62"/>
+      <c r="BG374" s="61"/>
       <c r="BH374" s="46"/>
-      <c r="BI374" s="62"/>
+      <c r="BI374" s="61"/>
       <c r="BJ374" s="46"/>
-      <c r="BK374" s="62"/>
+      <c r="BK374" s="61"/>
       <c r="BL374" s="46"/>
-      <c r="BM374" s="62"/>
+      <c r="BM374" s="61"/>
       <c r="BN374" s="46"/>
-      <c r="BO374" s="62"/>
+      <c r="BO374" s="61"/>
       <c r="BP374" s="46"/>
-      <c r="BQ374" s="62"/>
+      <c r="BQ374" s="61"/>
       <c r="BR374" s="46"/>
       <c r="BS374" s="42">
         <f t="shared" si="20"/>
@@ -79400,7 +79426,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW375" s="63" t="s">
+      <c r="BW375" s="62" t="s">
         <v>43</v>
       </c>
     </row>
@@ -79629,7 +79655,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW376" s="64" t="s">
+      <c r="BW376" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -79858,7 +79884,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW377" s="64" t="s">
+      <c r="BW377" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -80087,7 +80113,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW378" s="64" t="s">
+      <c r="BW378" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -80316,7 +80342,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW379" s="64" t="s">
+      <c r="BW379" s="63" t="s">
         <v>251</v>
       </c>
     </row>
@@ -80545,7 +80571,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW380" s="64" t="s">
+      <c r="BW380" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -80774,7 +80800,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW381" s="64" t="s">
+      <c r="BW381" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -81003,7 +81029,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW382" s="64" t="s">
+      <c r="BW382" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -81232,7 +81258,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW383" s="64" t="s">
+      <c r="BW383" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -81243,73 +81269,73 @@
       <c r="B384" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="C384" s="65"/>
+      <c r="C384" s="64"/>
       <c r="D384" s="46"/>
-      <c r="E384" s="65"/>
+      <c r="E384" s="64"/>
       <c r="F384" s="46"/>
-      <c r="G384" s="65"/>
+      <c r="G384" s="64"/>
       <c r="H384" s="46"/>
-      <c r="I384" s="65"/>
+      <c r="I384" s="64"/>
       <c r="J384" s="46"/>
-      <c r="K384" s="65"/>
+      <c r="K384" s="64"/>
       <c r="L384" s="46"/>
-      <c r="M384" s="65"/>
+      <c r="M384" s="64"/>
       <c r="N384" s="46"/>
-      <c r="O384" s="65"/>
+      <c r="O384" s="64"/>
       <c r="P384" s="46"/>
-      <c r="Q384" s="65"/>
+      <c r="Q384" s="64"/>
       <c r="R384" s="46"/>
-      <c r="S384" s="65"/>
+      <c r="S384" s="64"/>
       <c r="T384" s="46"/>
-      <c r="U384" s="65"/>
+      <c r="U384" s="64"/>
       <c r="V384" s="46"/>
-      <c r="W384" s="65"/>
+      <c r="W384" s="64"/>
       <c r="X384" s="46"/>
-      <c r="Y384" s="65"/>
+      <c r="Y384" s="64"/>
       <c r="Z384" s="46"/>
-      <c r="AA384" s="65"/>
+      <c r="AA384" s="64"/>
       <c r="AB384" s="46"/>
-      <c r="AC384" s="65"/>
+      <c r="AC384" s="64"/>
       <c r="AD384" s="46"/>
-      <c r="AE384" s="65"/>
+      <c r="AE384" s="64"/>
       <c r="AF384" s="46"/>
-      <c r="AG384" s="65"/>
+      <c r="AG384" s="64"/>
       <c r="AH384" s="46"/>
-      <c r="AI384" s="65"/>
+      <c r="AI384" s="64"/>
       <c r="AJ384" s="46"/>
-      <c r="AK384" s="65"/>
+      <c r="AK384" s="64"/>
       <c r="AL384" s="46"/>
-      <c r="AM384" s="65"/>
+      <c r="AM384" s="64"/>
       <c r="AN384" s="46"/>
-      <c r="AO384" s="65"/>
+      <c r="AO384" s="64"/>
       <c r="AP384" s="46"/>
-      <c r="AQ384" s="65"/>
+      <c r="AQ384" s="64"/>
       <c r="AR384" s="46"/>
-      <c r="AS384" s="65"/>
+      <c r="AS384" s="64"/>
       <c r="AT384" s="46"/>
-      <c r="AU384" s="65"/>
+      <c r="AU384" s="64"/>
       <c r="AV384" s="46"/>
-      <c r="AW384" s="65"/>
+      <c r="AW384" s="64"/>
       <c r="AX384" s="46"/>
-      <c r="AY384" s="65"/>
+      <c r="AY384" s="64"/>
       <c r="AZ384" s="46"/>
-      <c r="BA384" s="65"/>
+      <c r="BA384" s="64"/>
       <c r="BB384" s="46"/>
-      <c r="BC384" s="65"/>
+      <c r="BC384" s="64"/>
       <c r="BD384" s="46"/>
-      <c r="BE384" s="65"/>
+      <c r="BE384" s="64"/>
       <c r="BF384" s="46"/>
-      <c r="BG384" s="65"/>
+      <c r="BG384" s="64"/>
       <c r="BH384" s="46"/>
-      <c r="BI384" s="65"/>
+      <c r="BI384" s="64"/>
       <c r="BJ384" s="46"/>
-      <c r="BK384" s="65"/>
+      <c r="BK384" s="64"/>
       <c r="BL384" s="46"/>
-      <c r="BM384" s="65"/>
+      <c r="BM384" s="64"/>
       <c r="BN384" s="46"/>
-      <c r="BO384" s="65"/>
+      <c r="BO384" s="64"/>
       <c r="BP384" s="46"/>
-      <c r="BQ384" s="65"/>
+      <c r="BQ384" s="64"/>
       <c r="BR384" s="46"/>
       <c r="BS384" s="42">
         <f t="shared" si="20"/>
@@ -81324,7 +81350,7 @@
         <v>0</v>
       </c>
       <c r="BV384" s="43"/>
-      <c r="BW384" s="66"/>
+      <c r="BW384" s="65"/>
     </row>
     <row r="385" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A385" s="27"/>
@@ -81551,7 +81577,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW385" s="64" t="s">
+      <c r="BW385" s="63" t="s">
         <v>252</v>
       </c>
     </row>
@@ -81780,7 +81806,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW386" s="64" t="s">
+      <c r="BW386" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -82009,7 +82035,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW387" s="64" t="s">
+      <c r="BW387" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -82020,139 +82046,139 @@
       <c r="B388" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="C388" s="65"/>
+      <c r="C388" s="64"/>
       <c r="D388" s="42">
         <v>0</v>
       </c>
-      <c r="E388" s="65"/>
+      <c r="E388" s="64"/>
       <c r="F388" s="42">
         <v>0</v>
       </c>
-      <c r="G388" s="65"/>
+      <c r="G388" s="64"/>
       <c r="H388" s="42">
         <v>0</v>
       </c>
-      <c r="I388" s="65"/>
+      <c r="I388" s="64"/>
       <c r="J388" s="42">
         <v>0</v>
       </c>
-      <c r="K388" s="65"/>
+      <c r="K388" s="64"/>
       <c r="L388" s="42">
         <v>0</v>
       </c>
-      <c r="M388" s="65"/>
+      <c r="M388" s="64"/>
       <c r="N388" s="42">
         <v>0</v>
       </c>
-      <c r="O388" s="65"/>
+      <c r="O388" s="64"/>
       <c r="P388" s="42">
         <v>0</v>
       </c>
-      <c r="Q388" s="65"/>
+      <c r="Q388" s="64"/>
       <c r="R388" s="42">
         <v>0</v>
       </c>
-      <c r="S388" s="65"/>
+      <c r="S388" s="64"/>
       <c r="T388" s="42">
         <v>0</v>
       </c>
-      <c r="U388" s="65"/>
+      <c r="U388" s="64"/>
       <c r="V388" s="42">
         <v>0</v>
       </c>
-      <c r="W388" s="65"/>
+      <c r="W388" s="64"/>
       <c r="X388" s="42">
         <v>0</v>
       </c>
-      <c r="Y388" s="65"/>
+      <c r="Y388" s="64"/>
       <c r="Z388" s="42">
         <v>0</v>
       </c>
-      <c r="AA388" s="65"/>
+      <c r="AA388" s="64"/>
       <c r="AB388" s="42">
         <v>0</v>
       </c>
-      <c r="AC388" s="65"/>
+      <c r="AC388" s="64"/>
       <c r="AD388" s="42">
         <v>0</v>
       </c>
-      <c r="AE388" s="65"/>
+      <c r="AE388" s="64"/>
       <c r="AF388" s="42">
         <v>0</v>
       </c>
-      <c r="AG388" s="65"/>
+      <c r="AG388" s="64"/>
       <c r="AH388" s="42">
         <v>0</v>
       </c>
-      <c r="AI388" s="65"/>
+      <c r="AI388" s="64"/>
       <c r="AJ388" s="42">
         <v>0</v>
       </c>
-      <c r="AK388" s="65"/>
+      <c r="AK388" s="64"/>
       <c r="AL388" s="42">
         <v>0</v>
       </c>
-      <c r="AM388" s="65"/>
+      <c r="AM388" s="64"/>
       <c r="AN388" s="42">
         <v>0</v>
       </c>
-      <c r="AO388" s="65"/>
+      <c r="AO388" s="64"/>
       <c r="AP388" s="42">
         <v>0</v>
       </c>
-      <c r="AQ388" s="65"/>
+      <c r="AQ388" s="64"/>
       <c r="AR388" s="42">
         <v>0</v>
       </c>
-      <c r="AS388" s="65"/>
+      <c r="AS388" s="64"/>
       <c r="AT388" s="42">
         <v>0</v>
       </c>
-      <c r="AU388" s="65"/>
+      <c r="AU388" s="64"/>
       <c r="AV388" s="42">
         <v>0</v>
       </c>
-      <c r="AW388" s="65"/>
+      <c r="AW388" s="64"/>
       <c r="AX388" s="42">
         <v>0</v>
       </c>
-      <c r="AY388" s="65"/>
+      <c r="AY388" s="64"/>
       <c r="AZ388" s="42">
         <v>0</v>
       </c>
-      <c r="BA388" s="65"/>
+      <c r="BA388" s="64"/>
       <c r="BB388" s="42">
         <v>0</v>
       </c>
-      <c r="BC388" s="65"/>
+      <c r="BC388" s="64"/>
       <c r="BD388" s="42">
         <v>0</v>
       </c>
-      <c r="BE388" s="65"/>
+      <c r="BE388" s="64"/>
       <c r="BF388" s="42">
         <v>0</v>
       </c>
-      <c r="BG388" s="65"/>
+      <c r="BG388" s="64"/>
       <c r="BH388" s="42">
         <v>0</v>
       </c>
-      <c r="BI388" s="65"/>
+      <c r="BI388" s="64"/>
       <c r="BJ388" s="42">
         <v>0</v>
       </c>
-      <c r="BK388" s="65"/>
+      <c r="BK388" s="64"/>
       <c r="BL388" s="42">
         <v>0</v>
       </c>
-      <c r="BM388" s="65"/>
+      <c r="BM388" s="64"/>
       <c r="BN388" s="42">
         <v>0</v>
       </c>
-      <c r="BO388" s="65"/>
+      <c r="BO388" s="64"/>
       <c r="BP388" s="42">
         <v>0</v>
       </c>
-      <c r="BQ388" s="65"/>
+      <c r="BQ388" s="64"/>
       <c r="BR388" s="42">
         <v>0</v>
       </c>
@@ -82169,7 +82195,7 @@
         <v>0</v>
       </c>
       <c r="BV388" s="43"/>
-      <c r="BW388" s="67"/>
+      <c r="BW388" s="66"/>
     </row>
     <row r="389" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A389" s="27"/>
@@ -82396,7 +82422,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW389" s="64" t="s">
+      <c r="BW389" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -82625,7 +82651,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW390" s="64" t="s">
+      <c r="BW390" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -82854,7 +82880,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW391" s="64" t="s">
+      <c r="BW391" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -83083,7 +83109,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW392" s="64" t="s">
+      <c r="BW392" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -83312,7 +83338,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW393" s="64" t="s">
+      <c r="BW393" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -83541,7 +83567,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW394" s="64" t="s">
+      <c r="BW394" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -83770,7 +83796,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW395" s="64" t="s">
+      <c r="BW395" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -83999,7 +84025,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW396" s="64" t="s">
+      <c r="BW396" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -84228,7 +84254,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW397" s="68" t="s">
+      <c r="BW397" s="67" t="s">
         <v>327</v>
       </c>
     </row>
@@ -84457,7 +84483,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW398" s="64" t="s">
+      <c r="BW398" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -84686,7 +84712,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW399" s="64" t="s">
+      <c r="BW399" s="63" t="s">
         <v>43</v>
       </c>
     </row>
@@ -84915,7 +84941,7 @@
         <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW400" s="64" t="s">
+      <c r="BW400" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -85144,7 +85170,7 @@
         <f t="shared" ref="BV401:BV407" si="27">SUM(BT401-BS401)/BS401*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW401" s="64" t="s">
+      <c r="BW401" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -85155,73 +85181,73 @@
       <c r="B402" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="C402" s="65"/>
+      <c r="C402" s="64"/>
       <c r="D402" s="46"/>
-      <c r="E402" s="65"/>
+      <c r="E402" s="64"/>
       <c r="F402" s="46"/>
-      <c r="G402" s="65"/>
+      <c r="G402" s="64"/>
       <c r="H402" s="46"/>
-      <c r="I402" s="65"/>
+      <c r="I402" s="64"/>
       <c r="J402" s="46"/>
-      <c r="K402" s="65"/>
+      <c r="K402" s="64"/>
       <c r="L402" s="46"/>
-      <c r="M402" s="65"/>
+      <c r="M402" s="64"/>
       <c r="N402" s="46"/>
-      <c r="O402" s="65"/>
+      <c r="O402" s="64"/>
       <c r="P402" s="46"/>
-      <c r="Q402" s="65"/>
+      <c r="Q402" s="64"/>
       <c r="R402" s="46"/>
-      <c r="S402" s="65"/>
+      <c r="S402" s="64"/>
       <c r="T402" s="46"/>
-      <c r="U402" s="65"/>
+      <c r="U402" s="64"/>
       <c r="V402" s="46"/>
-      <c r="W402" s="65"/>
+      <c r="W402" s="64"/>
       <c r="X402" s="46"/>
-      <c r="Y402" s="65"/>
+      <c r="Y402" s="64"/>
       <c r="Z402" s="46"/>
-      <c r="AA402" s="65"/>
+      <c r="AA402" s="64"/>
       <c r="AB402" s="46"/>
-      <c r="AC402" s="65"/>
+      <c r="AC402" s="64"/>
       <c r="AD402" s="46"/>
-      <c r="AE402" s="65"/>
+      <c r="AE402" s="64"/>
       <c r="AF402" s="46"/>
-      <c r="AG402" s="65"/>
+      <c r="AG402" s="64"/>
       <c r="AH402" s="46"/>
-      <c r="AI402" s="65"/>
+      <c r="AI402" s="64"/>
       <c r="AJ402" s="46"/>
-      <c r="AK402" s="65"/>
+      <c r="AK402" s="64"/>
       <c r="AL402" s="46"/>
-      <c r="AM402" s="65"/>
+      <c r="AM402" s="64"/>
       <c r="AN402" s="46"/>
-      <c r="AO402" s="65"/>
+      <c r="AO402" s="64"/>
       <c r="AP402" s="46"/>
-      <c r="AQ402" s="65"/>
+      <c r="AQ402" s="64"/>
       <c r="AR402" s="46"/>
-      <c r="AS402" s="65"/>
+      <c r="AS402" s="64"/>
       <c r="AT402" s="46"/>
-      <c r="AU402" s="65"/>
+      <c r="AU402" s="64"/>
       <c r="AV402" s="46"/>
-      <c r="AW402" s="65"/>
+      <c r="AW402" s="64"/>
       <c r="AX402" s="46"/>
-      <c r="AY402" s="65"/>
+      <c r="AY402" s="64"/>
       <c r="AZ402" s="46"/>
-      <c r="BA402" s="65"/>
+      <c r="BA402" s="64"/>
       <c r="BB402" s="46"/>
-      <c r="BC402" s="65"/>
+      <c r="BC402" s="64"/>
       <c r="BD402" s="46"/>
-      <c r="BE402" s="65"/>
+      <c r="BE402" s="64"/>
       <c r="BF402" s="46"/>
-      <c r="BG402" s="65"/>
+      <c r="BG402" s="64"/>
       <c r="BH402" s="46"/>
-      <c r="BI402" s="65"/>
+      <c r="BI402" s="64"/>
       <c r="BJ402" s="46"/>
-      <c r="BK402" s="65"/>
+      <c r="BK402" s="64"/>
       <c r="BL402" s="46"/>
-      <c r="BM402" s="65"/>
+      <c r="BM402" s="64"/>
       <c r="BN402" s="46"/>
-      <c r="BO402" s="65"/>
+      <c r="BO402" s="64"/>
       <c r="BP402" s="46"/>
-      <c r="BQ402" s="65"/>
+      <c r="BQ402" s="64"/>
       <c r="BR402" s="46"/>
       <c r="BS402" s="42">
         <f t="shared" si="24"/>
@@ -85236,7 +85262,7 @@
         <v>0</v>
       </c>
       <c r="BV402" s="43"/>
-      <c r="BW402" s="67"/>
+      <c r="BW402" s="66"/>
     </row>
     <row r="403" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A403" s="27"/>
@@ -85463,7 +85489,7 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW403" s="64" t="s">
+      <c r="BW403" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -85692,7 +85718,7 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW404" s="64" t="s">
+      <c r="BW404" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -85921,7 +85947,7 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW405" s="64" t="s">
+      <c r="BW405" s="63" t="s">
         <v>261</v>
       </c>
     </row>
@@ -86150,7 +86176,7 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW406" s="64" t="s">
+      <c r="BW406" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -86379,7 +86405,7 @@
         <f t="shared" si="27"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BW407" s="64" t="s">
+      <c r="BW407" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -86390,73 +86416,73 @@
       <c r="B408" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="C408" s="60"/>
+      <c r="C408" s="59"/>
       <c r="D408" s="46"/>
-      <c r="E408" s="60"/>
+      <c r="E408" s="59"/>
       <c r="F408" s="46"/>
-      <c r="G408" s="60"/>
+      <c r="G408" s="59"/>
       <c r="H408" s="46"/>
-      <c r="I408" s="60"/>
+      <c r="I408" s="59"/>
       <c r="J408" s="46"/>
-      <c r="K408" s="60"/>
+      <c r="K408" s="59"/>
       <c r="L408" s="46"/>
-      <c r="M408" s="60"/>
+      <c r="M408" s="59"/>
       <c r="N408" s="46"/>
-      <c r="O408" s="60"/>
+      <c r="O408" s="59"/>
       <c r="P408" s="46"/>
-      <c r="Q408" s="60"/>
+      <c r="Q408" s="59"/>
       <c r="R408" s="46"/>
-      <c r="S408" s="60"/>
+      <c r="S408" s="59"/>
       <c r="T408" s="46"/>
-      <c r="U408" s="60"/>
+      <c r="U408" s="59"/>
       <c r="V408" s="46"/>
-      <c r="W408" s="60"/>
+      <c r="W408" s="59"/>
       <c r="X408" s="46"/>
-      <c r="Y408" s="60"/>
+      <c r="Y408" s="59"/>
       <c r="Z408" s="46"/>
-      <c r="AA408" s="60"/>
+      <c r="AA408" s="59"/>
       <c r="AB408" s="46"/>
-      <c r="AC408" s="60"/>
+      <c r="AC408" s="59"/>
       <c r="AD408" s="46"/>
-      <c r="AE408" s="60"/>
+      <c r="AE408" s="59"/>
       <c r="AF408" s="46"/>
-      <c r="AG408" s="60"/>
+      <c r="AG408" s="59"/>
       <c r="AH408" s="46"/>
-      <c r="AI408" s="60"/>
+      <c r="AI408" s="59"/>
       <c r="AJ408" s="46"/>
-      <c r="AK408" s="60"/>
+      <c r="AK408" s="59"/>
       <c r="AL408" s="46"/>
-      <c r="AM408" s="60"/>
+      <c r="AM408" s="59"/>
       <c r="AN408" s="46"/>
-      <c r="AO408" s="60"/>
+      <c r="AO408" s="59"/>
       <c r="AP408" s="46"/>
-      <c r="AQ408" s="60"/>
+      <c r="AQ408" s="59"/>
       <c r="AR408" s="46"/>
-      <c r="AS408" s="60"/>
+      <c r="AS408" s="59"/>
       <c r="AT408" s="46"/>
-      <c r="AU408" s="60"/>
+      <c r="AU408" s="59"/>
       <c r="AV408" s="46"/>
-      <c r="AW408" s="60"/>
+      <c r="AW408" s="59"/>
       <c r="AX408" s="46"/>
-      <c r="AY408" s="60"/>
+      <c r="AY408" s="59"/>
       <c r="AZ408" s="46"/>
-      <c r="BA408" s="60"/>
+      <c r="BA408" s="59"/>
       <c r="BB408" s="46"/>
-      <c r="BC408" s="60"/>
+      <c r="BC408" s="59"/>
       <c r="BD408" s="46"/>
-      <c r="BE408" s="60"/>
+      <c r="BE408" s="59"/>
       <c r="BF408" s="46"/>
-      <c r="BG408" s="60"/>
+      <c r="BG408" s="59"/>
       <c r="BH408" s="46"/>
-      <c r="BI408" s="60"/>
+      <c r="BI408" s="59"/>
       <c r="BJ408" s="46"/>
-      <c r="BK408" s="60"/>
+      <c r="BK408" s="59"/>
       <c r="BL408" s="46"/>
-      <c r="BM408" s="60"/>
+      <c r="BM408" s="59"/>
       <c r="BN408" s="46"/>
-      <c r="BO408" s="60"/>
+      <c r="BO408" s="59"/>
       <c r="BP408" s="46"/>
-      <c r="BQ408" s="60"/>
+      <c r="BQ408" s="59"/>
       <c r="BR408" s="46"/>
       <c r="BS408" s="42">
         <f t="shared" si="24"/>
@@ -86480,73 +86506,73 @@
       <c r="B409" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="C409" s="61"/>
+      <c r="C409" s="60"/>
       <c r="D409" s="46"/>
-      <c r="E409" s="61"/>
+      <c r="E409" s="60"/>
       <c r="F409" s="46"/>
-      <c r="G409" s="61"/>
+      <c r="G409" s="60"/>
       <c r="H409" s="46"/>
-      <c r="I409" s="61"/>
+      <c r="I409" s="60"/>
       <c r="J409" s="46"/>
-      <c r="K409" s="61"/>
+      <c r="K409" s="60"/>
       <c r="L409" s="46"/>
-      <c r="M409" s="61"/>
+      <c r="M409" s="60"/>
       <c r="N409" s="46"/>
-      <c r="O409" s="61"/>
+      <c r="O409" s="60"/>
       <c r="P409" s="46"/>
-      <c r="Q409" s="61"/>
+      <c r="Q409" s="60"/>
       <c r="R409" s="46"/>
-      <c r="S409" s="61"/>
+      <c r="S409" s="60"/>
       <c r="T409" s="46"/>
-      <c r="U409" s="61"/>
+      <c r="U409" s="60"/>
       <c r="V409" s="46"/>
-      <c r="W409" s="61"/>
+      <c r="W409" s="60"/>
       <c r="X409" s="46"/>
-      <c r="Y409" s="61"/>
+      <c r="Y409" s="60"/>
       <c r="Z409" s="46"/>
-      <c r="AA409" s="61"/>
+      <c r="AA409" s="60"/>
       <c r="AB409" s="46"/>
-      <c r="AC409" s="61"/>
+      <c r="AC409" s="60"/>
       <c r="AD409" s="46"/>
-      <c r="AE409" s="61"/>
+      <c r="AE409" s="60"/>
       <c r="AF409" s="46"/>
-      <c r="AG409" s="61"/>
+      <c r="AG409" s="60"/>
       <c r="AH409" s="46"/>
-      <c r="AI409" s="61"/>
+      <c r="AI409" s="60"/>
       <c r="AJ409" s="46"/>
-      <c r="AK409" s="61"/>
+      <c r="AK409" s="60"/>
       <c r="AL409" s="46"/>
-      <c r="AM409" s="61"/>
+      <c r="AM409" s="60"/>
       <c r="AN409" s="46"/>
-      <c r="AO409" s="61"/>
+      <c r="AO409" s="60"/>
       <c r="AP409" s="46"/>
-      <c r="AQ409" s="61"/>
+      <c r="AQ409" s="60"/>
       <c r="AR409" s="46"/>
-      <c r="AS409" s="61"/>
+      <c r="AS409" s="60"/>
       <c r="AT409" s="46"/>
-      <c r="AU409" s="61"/>
+      <c r="AU409" s="60"/>
       <c r="AV409" s="46"/>
-      <c r="AW409" s="61"/>
+      <c r="AW409" s="60"/>
       <c r="AX409" s="46"/>
-      <c r="AY409" s="61"/>
+      <c r="AY409" s="60"/>
       <c r="AZ409" s="46"/>
-      <c r="BA409" s="61"/>
+      <c r="BA409" s="60"/>
       <c r="BB409" s="46"/>
-      <c r="BC409" s="61"/>
+      <c r="BC409" s="60"/>
       <c r="BD409" s="46"/>
-      <c r="BE409" s="61"/>
+      <c r="BE409" s="60"/>
       <c r="BF409" s="46"/>
-      <c r="BG409" s="61"/>
+      <c r="BG409" s="60"/>
       <c r="BH409" s="46"/>
-      <c r="BI409" s="61"/>
+      <c r="BI409" s="60"/>
       <c r="BJ409" s="46"/>
-      <c r="BK409" s="61"/>
+      <c r="BK409" s="60"/>
       <c r="BL409" s="46"/>
-      <c r="BM409" s="61"/>
+      <c r="BM409" s="60"/>
       <c r="BN409" s="46"/>
-      <c r="BO409" s="61"/>
+      <c r="BO409" s="60"/>
       <c r="BP409" s="46"/>
-      <c r="BQ409" s="61"/>
+      <c r="BQ409" s="60"/>
       <c r="BR409" s="46"/>
       <c r="BS409" s="42">
         <f t="shared" si="24"/>
@@ -87484,275 +87510,275 @@
       <c r="B414" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C414" s="69">
+      <c r="C414" s="68">
         <f t="shared" ref="C414:BN414" si="29">SUM(C409:C413)</f>
         <v>0</v>
       </c>
-      <c r="D414" s="70">
+      <c r="D414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="E414" s="69">
+      <c r="E414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="F414" s="70">
+      <c r="F414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="G414" s="69">
+      <c r="G414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="H414" s="70">
+      <c r="H414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="I414" s="69">
+      <c r="I414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="J414" s="70">
+      <c r="J414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="K414" s="69">
+      <c r="K414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="L414" s="70">
+      <c r="L414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="M414" s="69">
+      <c r="M414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="N414" s="70">
+      <c r="N414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="O414" s="69">
+      <c r="O414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="P414" s="70">
+      <c r="P414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="Q414" s="69">
+      <c r="Q414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="R414" s="70">
+      <c r="R414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="S414" s="69">
+      <c r="S414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="T414" s="70">
+      <c r="T414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="U414" s="69">
+      <c r="U414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="V414" s="70">
+      <c r="V414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="W414" s="69">
+      <c r="W414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="X414" s="70">
+      <c r="X414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="Y414" s="69">
+      <c r="Y414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="Z414" s="70">
+      <c r="Z414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AA414" s="69">
+      <c r="AA414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AB414" s="70">
+      <c r="AB414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AC414" s="69">
+      <c r="AC414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AD414" s="70">
+      <c r="AD414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AE414" s="69">
+      <c r="AE414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AF414" s="70">
+      <c r="AF414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AG414" s="69">
+      <c r="AG414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AH414" s="70">
+      <c r="AH414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AI414" s="69">
+      <c r="AI414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AJ414" s="70">
+      <c r="AJ414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AK414" s="69">
+      <c r="AK414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AL414" s="70">
+      <c r="AL414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AM414" s="69">
+      <c r="AM414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AN414" s="70">
+      <c r="AN414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AO414" s="69">
+      <c r="AO414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AP414" s="70">
+      <c r="AP414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AQ414" s="69">
+      <c r="AQ414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AR414" s="70">
+      <c r="AR414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AS414" s="69">
+      <c r="AS414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AT414" s="70">
+      <c r="AT414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AU414" s="69">
+      <c r="AU414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AV414" s="70">
+      <c r="AV414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AW414" s="69">
+      <c r="AW414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AX414" s="70">
+      <c r="AX414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AY414" s="69">
+      <c r="AY414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AZ414" s="70">
+      <c r="AZ414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BA414" s="69">
+      <c r="BA414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BB414" s="70">
+      <c r="BB414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BC414" s="69">
+      <c r="BC414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BD414" s="70">
+      <c r="BD414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BE414" s="69">
+      <c r="BE414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BF414" s="70">
+      <c r="BF414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BG414" s="69">
+      <c r="BG414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BH414" s="70">
+      <c r="BH414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BI414" s="69">
+      <c r="BI414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BJ414" s="70">
+      <c r="BJ414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BK414" s="69">
+      <c r="BK414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BL414" s="70">
+      <c r="BL414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BM414" s="69">
+      <c r="BM414" s="68">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BN414" s="70">
+      <c r="BN414" s="69">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="BO414" s="69">
+      <c r="BO414" s="68">
         <f t="shared" ref="BO414:BR414" si="30">SUM(BO409:BO413)</f>
         <v>0</v>
       </c>
-      <c r="BP414" s="70">
+      <c r="BP414" s="69">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="BQ414" s="69">
+      <c r="BQ414" s="68">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="BR414" s="70">
+      <c r="BR414" s="69">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
@@ -87768,7 +87794,7 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="BV414" s="71" t="e">
+      <c r="BV414" s="70" t="e">
         <f>SUM(BT414-BS414)/BS414*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -87781,9 +87807,9 @@
       <c r="B415" s="30"/>
       <c r="C415" s="55"/>
       <c r="D415" s="55"/>
-      <c r="E415" s="73"/>
-      <c r="F415" s="73"/>
-      <c r="G415" s="73"/>
+      <c r="E415" s="74"/>
+      <c r="F415" s="74"/>
+      <c r="G415" s="74"/>
     </row>
     <row r="416" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A416" s="30"/>
@@ -87794,7 +87820,7 @@
       <c r="F416" s="55"/>
       <c r="G416" s="55"/>
     </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A417" s="30"/>
       <c r="B417" s="30"/>
       <c r="C417" s="55"/>
@@ -87802,8 +87828,12 @@
       <c r="E417" s="55"/>
       <c r="F417" s="55"/>
       <c r="G417" s="55"/>
+      <c r="BT417" s="82"/>
+      <c r="BU417" s="82"/>
+      <c r="BV417" s="82"/>
+      <c r="BW417" s="82"/>
     </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A418" s="30"/>
       <c r="B418" s="30"/>
       <c r="C418" s="55"/>
@@ -87811,8 +87841,12 @@
       <c r="E418" s="55"/>
       <c r="F418" s="55"/>
       <c r="G418" s="55"/>
+      <c r="BT418" s="77"/>
+      <c r="BU418" s="77"/>
+      <c r="BV418" s="77"/>
+      <c r="BW418" s="77"/>
     </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A419" s="30"/>
       <c r="B419" s="30"/>
       <c r="C419" s="55"/>
@@ -87821,7 +87855,7 @@
       <c r="F419" s="55"/>
       <c r="G419" s="55"/>
     </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A420" s="30"/>
       <c r="B420" s="30"/>
       <c r="C420" s="55"/>
@@ -87830,7 +87864,7 @@
       <c r="F420" s="55"/>
       <c r="G420" s="55"/>
     </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A421" s="30"/>
       <c r="B421" s="30"/>
       <c r="C421" s="55"/>
@@ -87839,7 +87873,7 @@
       <c r="F421" s="55"/>
       <c r="G421" s="55"/>
     </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:75" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A422" s="30"/>
       <c r="B422" s="30"/>
       <c r="C422" s="55"/>
@@ -87847,8 +87881,12 @@
       <c r="E422" s="55"/>
       <c r="F422" s="55"/>
       <c r="G422" s="55"/>
+      <c r="BT422" s="84"/>
+      <c r="BU422" s="84"/>
+      <c r="BV422" s="84"/>
+      <c r="BW422" s="84"/>
     </row>
-    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:75" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A423" s="30"/>
       <c r="B423" s="30"/>
       <c r="C423" s="55"/>
@@ -87856,8 +87894,12 @@
       <c r="E423" s="55"/>
       <c r="F423" s="55"/>
       <c r="G423" s="55"/>
+      <c r="BT423" s="83"/>
+      <c r="BU423" s="83"/>
+      <c r="BV423" s="83"/>
+      <c r="BW423" s="83"/>
     </row>
-    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A424" s="30"/>
       <c r="B424" s="30"/>
       <c r="C424" s="55"/>
@@ -87866,7 +87908,7 @@
       <c r="F424" s="55"/>
       <c r="G424" s="55"/>
     </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A425" s="30"/>
       <c r="B425" s="30"/>
       <c r="C425" s="55"/>
@@ -87875,7 +87917,7 @@
       <c r="F425" s="55"/>
       <c r="G425" s="55"/>
     </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A426" s="30"/>
       <c r="B426" s="30"/>
       <c r="C426" s="55"/>
@@ -87884,7 +87926,7 @@
       <c r="F426" s="55"/>
       <c r="G426" s="55"/>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A427" s="30"/>
       <c r="B427" s="30"/>
       <c r="C427" s="55"/>
@@ -87893,7 +87935,7 @@
       <c r="F427" s="55"/>
       <c r="G427" s="55"/>
     </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A428" s="30"/>
       <c r="B428" s="30"/>
       <c r="C428" s="55"/>
@@ -87902,7 +87944,7 @@
       <c r="F428" s="55"/>
       <c r="G428" s="55"/>
     </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A429" s="30"/>
       <c r="B429" s="30"/>
       <c r="C429" s="55"/>
@@ -87911,7 +87953,7 @@
       <c r="F429" s="55"/>
       <c r="G429" s="55"/>
     </row>
-    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A430" s="30"/>
       <c r="B430" s="30"/>
       <c r="C430" s="55"/>
@@ -87920,7 +87962,7 @@
       <c r="F430" s="55"/>
       <c r="G430" s="55"/>
     </row>
-    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A431" s="30"/>
       <c r="B431" s="30"/>
       <c r="C431" s="55"/>
@@ -87929,7 +87971,7 @@
       <c r="F431" s="55"/>
       <c r="G431" s="55"/>
     </row>
-    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A432" s="30"/>
       <c r="B432" s="30"/>
       <c r="C432" s="55"/>
@@ -88236,7 +88278,11 @@
       <c r="G465" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="85">
+    <mergeCell ref="BT417:BW417"/>
+    <mergeCell ref="BT418:BW418"/>
+    <mergeCell ref="BT422:BW422"/>
+    <mergeCell ref="BT423:BW423"/>
     <mergeCell ref="BM8:BN8"/>
     <mergeCell ref="BO8:BP8"/>
     <mergeCell ref="BQ8:BR8"/>
@@ -88285,7 +88331,6 @@
     <mergeCell ref="BE9:BF9"/>
     <mergeCell ref="AM9:AN9"/>
     <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="AQ9:AR9"/>
     <mergeCell ref="AS9:AT9"/>
     <mergeCell ref="AU9:AV9"/>
     <mergeCell ref="AC9:AD9"/>
@@ -88293,23 +88338,7 @@
     <mergeCell ref="AG9:AH9"/>
     <mergeCell ref="AI9:AJ9"/>
     <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E415:G415"/>
-    <mergeCell ref="A7:G7"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A5:G5"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
@@ -88318,6 +88347,23 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:BW5"/>
+    <mergeCell ref="A6:BW6"/>
+    <mergeCell ref="A7:BW7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="E415:G415"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AQ9:AR9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.31496062992125984" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Fix compareAllPoldaInput function template
</commit_message>
<xml_diff>
--- a/public/template/excel/format_laporan_detail_daily.xlsx
+++ b/public/template/excel/format_laporan_detail_daily.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="330">
   <si>
     <t>URAIAN</t>
   </si>
@@ -938,9 +938,6 @@
     <t xml:space="preserve">KESATUAN :  </t>
   </si>
   <si>
-    <t xml:space="preserve">HARI/TGL : </t>
-  </si>
-  <si>
     <t>LAPORAN HARIAN OPS KESELAMATAN TAHUN 2020</t>
   </si>
   <si>
@@ -1655,20 +1652,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1679,16 +1685,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2058,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW465"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="AX408" zoomScale="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="BT423" sqref="BT423:BW423"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:BW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2076,566 +2073,564 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
-        <v>328</v>
-      </c>
-      <c r="B1" s="75"/>
+      <c r="A1" s="79" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" s="79"/>
     </row>
     <row r="2" spans="1:75" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
-        <v>329</v>
-      </c>
-      <c r="B2" s="75"/>
+      <c r="A2" s="79" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="79"/>
       <c r="C2" s="72"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
-        <v>330</v>
-      </c>
-      <c r="B3" s="77"/>
+      <c r="A3" s="74" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="74"/>
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="78"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="78"/>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78"/>
-      <c r="AK5" s="78"/>
-      <c r="AL5" s="78"/>
-      <c r="AM5" s="78"/>
-      <c r="AN5" s="78"/>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="78"/>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="78"/>
-      <c r="AW5" s="78"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="78"/>
-      <c r="AZ5" s="78"/>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="78"/>
-      <c r="BC5" s="78"/>
-      <c r="BD5" s="78"/>
-      <c r="BE5" s="78"/>
-      <c r="BF5" s="78"/>
-      <c r="BG5" s="78"/>
-      <c r="BH5" s="78"/>
-      <c r="BI5" s="78"/>
-      <c r="BJ5" s="78"/>
-      <c r="BK5" s="78"/>
-      <c r="BL5" s="78"/>
-      <c r="BM5" s="78"/>
-      <c r="BN5" s="78"/>
-      <c r="BO5" s="78"/>
-      <c r="BP5" s="78"/>
-      <c r="BQ5" s="78"/>
-      <c r="BR5" s="78"/>
-      <c r="BS5" s="78"/>
-      <c r="BT5" s="78"/>
-      <c r="BU5" s="78"/>
-      <c r="BV5" s="78"/>
-      <c r="BW5" s="78"/>
+      <c r="A5" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="81"/>
+      <c r="AG5" s="81"/>
+      <c r="AH5" s="81"/>
+      <c r="AI5" s="81"/>
+      <c r="AJ5" s="81"/>
+      <c r="AK5" s="81"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="81"/>
+      <c r="AN5" s="81"/>
+      <c r="AO5" s="81"/>
+      <c r="AP5" s="81"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="81"/>
+      <c r="AS5" s="81"/>
+      <c r="AT5" s="81"/>
+      <c r="AU5" s="81"/>
+      <c r="AV5" s="81"/>
+      <c r="AW5" s="81"/>
+      <c r="AX5" s="81"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="81"/>
+      <c r="BA5" s="81"/>
+      <c r="BB5" s="81"/>
+      <c r="BC5" s="81"/>
+      <c r="BD5" s="81"/>
+      <c r="BE5" s="81"/>
+      <c r="BF5" s="81"/>
+      <c r="BG5" s="81"/>
+      <c r="BH5" s="81"/>
+      <c r="BI5" s="81"/>
+      <c r="BJ5" s="81"/>
+      <c r="BK5" s="81"/>
+      <c r="BL5" s="81"/>
+      <c r="BM5" s="81"/>
+      <c r="BN5" s="81"/>
+      <c r="BO5" s="81"/>
+      <c r="BP5" s="81"/>
+      <c r="BQ5" s="81"/>
+      <c r="BR5" s="81"/>
+      <c r="BS5" s="81"/>
+      <c r="BT5" s="81"/>
+      <c r="BU5" s="81"/>
+      <c r="BV5" s="81"/>
+      <c r="BW5" s="81"/>
     </row>
     <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="82" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
-      <c r="S6" s="79"/>
-      <c r="T6" s="79"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="79"/>
-      <c r="X6" s="79"/>
-      <c r="Y6" s="79"/>
-      <c r="Z6" s="79"/>
-      <c r="AA6" s="79"/>
-      <c r="AB6" s="79"/>
-      <c r="AC6" s="79"/>
-      <c r="AD6" s="79"/>
-      <c r="AE6" s="79"/>
-      <c r="AF6" s="79"/>
-      <c r="AG6" s="79"/>
-      <c r="AH6" s="79"/>
-      <c r="AI6" s="79"/>
-      <c r="AJ6" s="79"/>
-      <c r="AK6" s="79"/>
-      <c r="AL6" s="79"/>
-      <c r="AM6" s="79"/>
-      <c r="AN6" s="79"/>
-      <c r="AO6" s="79"/>
-      <c r="AP6" s="79"/>
-      <c r="AQ6" s="79"/>
-      <c r="AR6" s="79"/>
-      <c r="AS6" s="79"/>
-      <c r="AT6" s="79"/>
-      <c r="AU6" s="79"/>
-      <c r="AV6" s="79"/>
-      <c r="AW6" s="79"/>
-      <c r="AX6" s="79"/>
-      <c r="AY6" s="79"/>
-      <c r="AZ6" s="79"/>
-      <c r="BA6" s="79"/>
-      <c r="BB6" s="79"/>
-      <c r="BC6" s="79"/>
-      <c r="BD6" s="79"/>
-      <c r="BE6" s="79"/>
-      <c r="BF6" s="79"/>
-      <c r="BG6" s="79"/>
-      <c r="BH6" s="79"/>
-      <c r="BI6" s="79"/>
-      <c r="BJ6" s="79"/>
-      <c r="BK6" s="79"/>
-      <c r="BL6" s="79"/>
-      <c r="BM6" s="79"/>
-      <c r="BN6" s="79"/>
-      <c r="BO6" s="79"/>
-      <c r="BP6" s="79"/>
-      <c r="BQ6" s="79"/>
-      <c r="BR6" s="79"/>
-      <c r="BS6" s="79"/>
-      <c r="BT6" s="79"/>
-      <c r="BU6" s="79"/>
-      <c r="BV6" s="79"/>
-      <c r="BW6" s="79"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="82"/>
+      <c r="Y6" s="82"/>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="82"/>
+      <c r="AB6" s="82"/>
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="82"/>
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="82"/>
+      <c r="AH6" s="82"/>
+      <c r="AI6" s="82"/>
+      <c r="AJ6" s="82"/>
+      <c r="AK6" s="82"/>
+      <c r="AL6" s="82"/>
+      <c r="AM6" s="82"/>
+      <c r="AN6" s="82"/>
+      <c r="AO6" s="82"/>
+      <c r="AP6" s="82"/>
+      <c r="AQ6" s="82"/>
+      <c r="AR6" s="82"/>
+      <c r="AS6" s="82"/>
+      <c r="AT6" s="82"/>
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="82"/>
+      <c r="AW6" s="82"/>
+      <c r="AX6" s="82"/>
+      <c r="AY6" s="82"/>
+      <c r="AZ6" s="82"/>
+      <c r="BA6" s="82"/>
+      <c r="BB6" s="82"/>
+      <c r="BC6" s="82"/>
+      <c r="BD6" s="82"/>
+      <c r="BE6" s="82"/>
+      <c r="BF6" s="82"/>
+      <c r="BG6" s="82"/>
+      <c r="BH6" s="82"/>
+      <c r="BI6" s="82"/>
+      <c r="BJ6" s="82"/>
+      <c r="BK6" s="82"/>
+      <c r="BL6" s="82"/>
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="82"/>
+      <c r="BO6" s="82"/>
+      <c r="BP6" s="82"/>
+      <c r="BQ6" s="82"/>
+      <c r="BR6" s="82"/>
+      <c r="BS6" s="82"/>
+      <c r="BT6" s="82"/>
+      <c r="BU6" s="82"/>
+      <c r="BV6" s="82"/>
+      <c r="BW6" s="82"/>
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
-        <v>278</v>
-      </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="80"/>
-      <c r="S7" s="80"/>
-      <c r="T7" s="80"/>
-      <c r="U7" s="80"/>
-      <c r="V7" s="80"/>
-      <c r="W7" s="80"/>
-      <c r="X7" s="80"/>
-      <c r="Y7" s="80"/>
-      <c r="Z7" s="80"/>
-      <c r="AA7" s="80"/>
-      <c r="AB7" s="80"/>
-      <c r="AC7" s="80"/>
-      <c r="AD7" s="80"/>
-      <c r="AE7" s="80"/>
-      <c r="AF7" s="80"/>
-      <c r="AG7" s="80"/>
-      <c r="AH7" s="80"/>
-      <c r="AI7" s="80"/>
-      <c r="AJ7" s="80"/>
-      <c r="AK7" s="80"/>
-      <c r="AL7" s="80"/>
-      <c r="AM7" s="80"/>
-      <c r="AN7" s="80"/>
-      <c r="AO7" s="80"/>
-      <c r="AP7" s="80"/>
-      <c r="AQ7" s="80"/>
-      <c r="AR7" s="80"/>
-      <c r="AS7" s="80"/>
-      <c r="AT7" s="80"/>
-      <c r="AU7" s="80"/>
-      <c r="AV7" s="80"/>
-      <c r="AW7" s="80"/>
-      <c r="AX7" s="80"/>
-      <c r="AY7" s="80"/>
-      <c r="AZ7" s="80"/>
-      <c r="BA7" s="80"/>
-      <c r="BB7" s="80"/>
-      <c r="BC7" s="80"/>
-      <c r="BD7" s="80"/>
-      <c r="BE7" s="80"/>
-      <c r="BF7" s="80"/>
-      <c r="BG7" s="80"/>
-      <c r="BH7" s="80"/>
-      <c r="BI7" s="80"/>
-      <c r="BJ7" s="80"/>
-      <c r="BK7" s="80"/>
-      <c r="BL7" s="80"/>
-      <c r="BM7" s="80"/>
-      <c r="BN7" s="80"/>
-      <c r="BO7" s="80"/>
-      <c r="BP7" s="80"/>
-      <c r="BQ7" s="80"/>
-      <c r="BR7" s="80"/>
-      <c r="BS7" s="80"/>
-      <c r="BT7" s="80"/>
-      <c r="BU7" s="80"/>
-      <c r="BV7" s="80"/>
-      <c r="BW7" s="80"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
+      <c r="AH7" s="83"/>
+      <c r="AI7" s="83"/>
+      <c r="AJ7" s="83"/>
+      <c r="AK7" s="83"/>
+      <c r="AL7" s="83"/>
+      <c r="AM7" s="83"/>
+      <c r="AN7" s="83"/>
+      <c r="AO7" s="83"/>
+      <c r="AP7" s="83"/>
+      <c r="AQ7" s="83"/>
+      <c r="AR7" s="83"/>
+      <c r="AS7" s="83"/>
+      <c r="AT7" s="83"/>
+      <c r="AU7" s="83"/>
+      <c r="AV7" s="83"/>
+      <c r="AW7" s="83"/>
+      <c r="AX7" s="83"/>
+      <c r="AY7" s="83"/>
+      <c r="AZ7" s="83"/>
+      <c r="BA7" s="83"/>
+      <c r="BB7" s="83"/>
+      <c r="BC7" s="83"/>
+      <c r="BD7" s="83"/>
+      <c r="BE7" s="83"/>
+      <c r="BF7" s="83"/>
+      <c r="BG7" s="83"/>
+      <c r="BH7" s="83"/>
+      <c r="BI7" s="83"/>
+      <c r="BJ7" s="83"/>
+      <c r="BK7" s="83"/>
+      <c r="BL7" s="83"/>
+      <c r="BM7" s="83"/>
+      <c r="BN7" s="83"/>
+      <c r="BO7" s="83"/>
+      <c r="BP7" s="83"/>
+      <c r="BQ7" s="83"/>
+      <c r="BR7" s="83"/>
+      <c r="BS7" s="83"/>
+      <c r="BT7" s="83"/>
+      <c r="BU7" s="83"/>
+      <c r="BV7" s="83"/>
+      <c r="BW7" s="83"/>
     </row>
     <row r="8" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
-        <v>326</v>
-      </c>
-      <c r="B8" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="73" t="s">
+      <c r="A8" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77" t="s">
         <v>291</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73" t="s">
+      <c r="F8" s="77"/>
+      <c r="G8" s="77" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73" t="s">
+      <c r="H8" s="77"/>
+      <c r="I8" s="77" t="s">
         <v>293</v>
       </c>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73" t="s">
+      <c r="J8" s="77"/>
+      <c r="K8" s="77" t="s">
         <v>294</v>
       </c>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73" t="s">
+      <c r="L8" s="77"/>
+      <c r="M8" s="77" t="s">
         <v>295</v>
       </c>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73" t="s">
+      <c r="N8" s="77"/>
+      <c r="O8" s="77" t="s">
         <v>296</v>
       </c>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73" t="s">
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77" t="s">
         <v>297</v>
       </c>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73" t="s">
+      <c r="R8" s="77"/>
+      <c r="S8" s="77" t="s">
         <v>298</v>
       </c>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73" t="s">
+      <c r="T8" s="77"/>
+      <c r="U8" s="77" t="s">
         <v>299</v>
       </c>
-      <c r="T8" s="73"/>
-      <c r="U8" s="73" t="s">
+      <c r="V8" s="77"/>
+      <c r="W8" s="77" t="s">
         <v>300</v>
       </c>
-      <c r="V8" s="73"/>
-      <c r="W8" s="73" t="s">
+      <c r="X8" s="77"/>
+      <c r="Y8" s="77" t="s">
         <v>301</v>
       </c>
-      <c r="X8" s="73"/>
-      <c r="Y8" s="73" t="s">
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="77" t="s">
         <v>302</v>
       </c>
-      <c r="Z8" s="73"/>
-      <c r="AA8" s="73" t="s">
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="77" t="s">
         <v>303</v>
       </c>
-      <c r="AB8" s="73"/>
-      <c r="AC8" s="73" t="s">
+      <c r="AD8" s="77"/>
+      <c r="AE8" s="77" t="s">
         <v>304</v>
       </c>
-      <c r="AD8" s="73"/>
-      <c r="AE8" s="73" t="s">
+      <c r="AF8" s="77"/>
+      <c r="AG8" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="AF8" s="73"/>
-      <c r="AG8" s="73" t="s">
+      <c r="AH8" s="77"/>
+      <c r="AI8" s="77" t="s">
         <v>306</v>
       </c>
-      <c r="AH8" s="73"/>
-      <c r="AI8" s="73" t="s">
+      <c r="AJ8" s="77"/>
+      <c r="AK8" s="77" t="s">
         <v>307</v>
       </c>
-      <c r="AJ8" s="73"/>
-      <c r="AK8" s="73" t="s">
+      <c r="AL8" s="77"/>
+      <c r="AM8" s="77" t="s">
         <v>308</v>
       </c>
-      <c r="AL8" s="73"/>
-      <c r="AM8" s="73" t="s">
+      <c r="AN8" s="77"/>
+      <c r="AO8" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="AN8" s="73"/>
-      <c r="AO8" s="73" t="s">
+      <c r="AP8" s="77"/>
+      <c r="AQ8" s="77" t="s">
         <v>310</v>
       </c>
-      <c r="AP8" s="73"/>
-      <c r="AQ8" s="73" t="s">
+      <c r="AR8" s="77"/>
+      <c r="AS8" s="77" t="s">
         <v>311</v>
       </c>
-      <c r="AR8" s="73"/>
-      <c r="AS8" s="73" t="s">
+      <c r="AT8" s="77"/>
+      <c r="AU8" s="77" t="s">
         <v>312</v>
       </c>
-      <c r="AT8" s="73"/>
-      <c r="AU8" s="73" t="s">
+      <c r="AV8" s="77"/>
+      <c r="AW8" s="77" t="s">
         <v>313</v>
       </c>
-      <c r="AV8" s="73"/>
-      <c r="AW8" s="73" t="s">
+      <c r="AX8" s="77"/>
+      <c r="AY8" s="77" t="s">
         <v>314</v>
       </c>
-      <c r="AX8" s="73"/>
-      <c r="AY8" s="73" t="s">
+      <c r="AZ8" s="77"/>
+      <c r="BA8" s="77" t="s">
         <v>315</v>
       </c>
-      <c r="AZ8" s="73"/>
-      <c r="BA8" s="73" t="s">
+      <c r="BB8" s="77"/>
+      <c r="BC8" s="78" t="s">
         <v>316</v>
       </c>
-      <c r="BB8" s="73"/>
-      <c r="BC8" s="81" t="s">
+      <c r="BD8" s="78"/>
+      <c r="BE8" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="BD8" s="81"/>
-      <c r="BE8" s="73" t="s">
+      <c r="BF8" s="77"/>
+      <c r="BG8" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="BF8" s="73"/>
-      <c r="BG8" s="73" t="s">
+      <c r="BH8" s="77"/>
+      <c r="BI8" s="77" t="s">
         <v>319</v>
       </c>
-      <c r="BH8" s="73"/>
-      <c r="BI8" s="73" t="s">
+      <c r="BJ8" s="77"/>
+      <c r="BK8" s="77" t="s">
         <v>320</v>
       </c>
-      <c r="BJ8" s="73"/>
-      <c r="BK8" s="73" t="s">
+      <c r="BL8" s="77"/>
+      <c r="BM8" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="BL8" s="73"/>
-      <c r="BM8" s="73" t="s">
+      <c r="BN8" s="77"/>
+      <c r="BO8" s="77" t="s">
         <v>322</v>
       </c>
-      <c r="BN8" s="73"/>
-      <c r="BO8" s="73" t="s">
+      <c r="BP8" s="77"/>
+      <c r="BQ8" s="77" t="s">
         <v>323</v>
       </c>
-      <c r="BP8" s="73"/>
-      <c r="BQ8" s="73" t="s">
+      <c r="BR8" s="77"/>
+      <c r="BS8" s="77" t="s">
         <v>324</v>
       </c>
-      <c r="BR8" s="73"/>
-      <c r="BS8" s="73" t="s">
-        <v>325</v>
-      </c>
-      <c r="BT8" s="73"/>
-      <c r="BU8" s="73"/>
-      <c r="BV8" s="73"/>
-      <c r="BW8" s="73" t="s">
+      <c r="BT8" s="77"/>
+      <c r="BU8" s="77"/>
+      <c r="BV8" s="77"/>
+      <c r="BW8" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="73" t="s">
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73" t="s">
+      <c r="D9" s="77"/>
+      <c r="E9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73" t="s">
+      <c r="F9" s="77"/>
+      <c r="G9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73" t="s">
+      <c r="H9" s="77"/>
+      <c r="I9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73" t="s">
+      <c r="J9" s="77"/>
+      <c r="K9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73" t="s">
+      <c r="L9" s="77"/>
+      <c r="M9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="N9" s="73"/>
-      <c r="O9" s="73" t="s">
+      <c r="N9" s="77"/>
+      <c r="O9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73" t="s">
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73" t="s">
+      <c r="R9" s="77"/>
+      <c r="S9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73" t="s">
+      <c r="T9" s="77"/>
+      <c r="U9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73" t="s">
+      <c r="V9" s="77"/>
+      <c r="W9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="X9" s="73"/>
-      <c r="Y9" s="73" t="s">
+      <c r="X9" s="77"/>
+      <c r="Y9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="Z9" s="73"/>
-      <c r="AA9" s="73" t="s">
+      <c r="Z9" s="77"/>
+      <c r="AA9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AB9" s="73"/>
-      <c r="AC9" s="73" t="s">
+      <c r="AB9" s="77"/>
+      <c r="AC9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AD9" s="73"/>
-      <c r="AE9" s="73" t="s">
+      <c r="AD9" s="77"/>
+      <c r="AE9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AF9" s="73"/>
-      <c r="AG9" s="73" t="s">
+      <c r="AF9" s="77"/>
+      <c r="AG9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AH9" s="73"/>
-      <c r="AI9" s="73" t="s">
+      <c r="AH9" s="77"/>
+      <c r="AI9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AJ9" s="73"/>
-      <c r="AK9" s="73" t="s">
+      <c r="AJ9" s="77"/>
+      <c r="AK9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AL9" s="73"/>
-      <c r="AM9" s="73" t="s">
+      <c r="AL9" s="77"/>
+      <c r="AM9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AN9" s="73"/>
-      <c r="AO9" s="73" t="s">
+      <c r="AN9" s="77"/>
+      <c r="AO9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AP9" s="73"/>
-      <c r="AQ9" s="73" t="s">
+      <c r="AP9" s="77"/>
+      <c r="AQ9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AR9" s="73"/>
-      <c r="AS9" s="73" t="s">
+      <c r="AR9" s="77"/>
+      <c r="AS9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AT9" s="73"/>
-      <c r="AU9" s="73" t="s">
+      <c r="AT9" s="77"/>
+      <c r="AU9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AV9" s="73"/>
-      <c r="AW9" s="73" t="s">
+      <c r="AV9" s="77"/>
+      <c r="AW9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AX9" s="73"/>
-      <c r="AY9" s="73" t="s">
+      <c r="AX9" s="77"/>
+      <c r="AY9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="AZ9" s="73"/>
-      <c r="BA9" s="73" t="s">
+      <c r="AZ9" s="77"/>
+      <c r="BA9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BB9" s="73"/>
-      <c r="BC9" s="81" t="s">
+      <c r="BB9" s="77"/>
+      <c r="BC9" s="78" t="s">
         <v>168</v>
       </c>
-      <c r="BD9" s="81"/>
-      <c r="BE9" s="73" t="s">
+      <c r="BD9" s="78"/>
+      <c r="BE9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BF9" s="73"/>
-      <c r="BG9" s="73" t="s">
+      <c r="BF9" s="77"/>
+      <c r="BG9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BH9" s="73"/>
-      <c r="BI9" s="73" t="s">
+      <c r="BH9" s="77"/>
+      <c r="BI9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BJ9" s="73"/>
-      <c r="BK9" s="73" t="s">
+      <c r="BJ9" s="77"/>
+      <c r="BK9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BL9" s="73"/>
-      <c r="BM9" s="73" t="s">
+      <c r="BL9" s="77"/>
+      <c r="BM9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BN9" s="73"/>
-      <c r="BO9" s="73" t="s">
+      <c r="BN9" s="77"/>
+      <c r="BO9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BP9" s="73"/>
-      <c r="BQ9" s="73" t="s">
+      <c r="BP9" s="77"/>
+      <c r="BQ9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BR9" s="73"/>
-      <c r="BS9" s="73" t="s">
+      <c r="BR9" s="77"/>
+      <c r="BS9" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="BT9" s="73"/>
-      <c r="BU9" s="73" t="s">
+      <c r="BT9" s="77"/>
+      <c r="BU9" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="BV9" s="73"/>
-      <c r="BW9" s="73"/>
+      <c r="BV9" s="77"/>
+      <c r="BW9" s="77"/>
     </row>
     <row r="10" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="39"/>
       <c r="D10" s="71"/>
       <c r="E10" s="71"/>
@@ -2712,7 +2707,7 @@
       <c r="BV10" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="BW10" s="73"/>
+      <c r="BW10" s="77"/>
     </row>
     <row r="11" spans="1:75" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="37">
@@ -72007,7 +72002,7 @@
     <row r="339" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A339" s="4"/>
       <c r="B339" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C339" s="42">
         <v>0</v>
@@ -72236,7 +72231,7 @@
     <row r="340" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A340" s="4"/>
       <c r="B340" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C340" s="42">
         <v>0</v>
@@ -72465,7 +72460,7 @@
     <row r="341" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A341" s="4"/>
       <c r="B341" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C341" s="42">
         <v>0</v>
@@ -72694,7 +72689,7 @@
     <row r="342" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A342" s="4"/>
       <c r="B342" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C342" s="42">
         <v>0</v>
@@ -84255,7 +84250,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="BW397" s="67" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="398" spans="1:75" x14ac:dyDescent="0.25">
@@ -86411,10 +86406,10 @@
     </row>
     <row r="408" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A408" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B408" s="35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C408" s="59"/>
       <c r="D408" s="46"/>
@@ -86504,7 +86499,7 @@
         <v>34</v>
       </c>
       <c r="B409" s="33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C409" s="60"/>
       <c r="D409" s="46"/>
@@ -86592,7 +86587,7 @@
     <row r="410" spans="1:75" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A410" s="27"/>
       <c r="B410" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C410" s="42">
         <v>0</v>
@@ -86821,7 +86816,7 @@
     <row r="411" spans="1:75" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A411" s="27"/>
       <c r="B411" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C411" s="42">
         <v>0</v>
@@ -87050,7 +87045,7 @@
     <row r="412" spans="1:75" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A412" s="27"/>
       <c r="B412" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C412" s="42">
         <v>0</v>
@@ -87279,7 +87274,7 @@
     <row r="413" spans="1:75" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A413" s="27"/>
       <c r="B413" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C413" s="42">
         <v>0</v>
@@ -87807,9 +87802,9 @@
       <c r="B415" s="30"/>
       <c r="C415" s="55"/>
       <c r="D415" s="55"/>
-      <c r="E415" s="74"/>
-      <c r="F415" s="74"/>
-      <c r="G415" s="74"/>
+      <c r="E415" s="84"/>
+      <c r="F415" s="84"/>
+      <c r="G415" s="84"/>
     </row>
     <row r="416" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A416" s="30"/>
@@ -87828,10 +87823,10 @@
       <c r="E417" s="55"/>
       <c r="F417" s="55"/>
       <c r="G417" s="55"/>
-      <c r="BT417" s="82"/>
-      <c r="BU417" s="82"/>
-      <c r="BV417" s="82"/>
-      <c r="BW417" s="82"/>
+      <c r="BT417" s="73"/>
+      <c r="BU417" s="73"/>
+      <c r="BV417" s="73"/>
+      <c r="BW417" s="73"/>
     </row>
     <row r="418" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A418" s="30"/>
@@ -87841,10 +87836,10 @@
       <c r="E418" s="55"/>
       <c r="F418" s="55"/>
       <c r="G418" s="55"/>
-      <c r="BT418" s="77"/>
-      <c r="BU418" s="77"/>
-      <c r="BV418" s="77"/>
-      <c r="BW418" s="77"/>
+      <c r="BT418" s="74"/>
+      <c r="BU418" s="74"/>
+      <c r="BV418" s="74"/>
+      <c r="BW418" s="74"/>
     </row>
     <row r="419" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A419" s="30"/>
@@ -87881,10 +87876,10 @@
       <c r="E422" s="55"/>
       <c r="F422" s="55"/>
       <c r="G422" s="55"/>
-      <c r="BT422" s="84"/>
-      <c r="BU422" s="84"/>
-      <c r="BV422" s="84"/>
-      <c r="BW422" s="84"/>
+      <c r="BT422" s="75"/>
+      <c r="BU422" s="75"/>
+      <c r="BV422" s="75"/>
+      <c r="BW422" s="75"/>
     </row>
     <row r="423" spans="1:75" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A423" s="30"/>
@@ -87894,10 +87889,10 @@
       <c r="E423" s="55"/>
       <c r="F423" s="55"/>
       <c r="G423" s="55"/>
-      <c r="BT423" s="83"/>
-      <c r="BU423" s="83"/>
-      <c r="BV423" s="83"/>
-      <c r="BW423" s="83"/>
+      <c r="BT423" s="76"/>
+      <c r="BU423" s="76"/>
+      <c r="BV423" s="76"/>
+      <c r="BW423" s="76"/>
     </row>
     <row r="424" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A424" s="30"/>
@@ -88279,42 +88274,39 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="BT417:BW417"/>
-    <mergeCell ref="BT418:BW418"/>
-    <mergeCell ref="BT422:BW422"/>
-    <mergeCell ref="BT423:BW423"/>
-    <mergeCell ref="BM8:BN8"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="BQ8:BR8"/>
-    <mergeCell ref="BS8:BV8"/>
-    <mergeCell ref="BW8:BW10"/>
-    <mergeCell ref="BS9:BT9"/>
-    <mergeCell ref="BU9:BV9"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="BE8:BF8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BI8:BJ8"/>
-    <mergeCell ref="BK8:BL8"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="AW8:AX8"/>
-    <mergeCell ref="AY8:AZ8"/>
-    <mergeCell ref="BA8:BB8"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AK8:AL8"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AG8:AH8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="E415:G415"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:BW5"/>
+    <mergeCell ref="A6:BW6"/>
+    <mergeCell ref="A7:BW7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AU9:AV9"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AI9:AJ9"/>
+    <mergeCell ref="AK9:AL9"/>
     <mergeCell ref="S8:T8"/>
     <mergeCell ref="U8:V8"/>
     <mergeCell ref="W8:X8"/>
@@ -88331,39 +88323,42 @@
     <mergeCell ref="BE9:BF9"/>
     <mergeCell ref="AM9:AN9"/>
     <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AU9:AV9"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AI9:AJ9"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:BW5"/>
-    <mergeCell ref="A6:BW6"/>
-    <mergeCell ref="A7:BW7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="E415:G415"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AG8:AH8"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="AW8:AX8"/>
+    <mergeCell ref="AY8:AZ8"/>
+    <mergeCell ref="BA8:BB8"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="BE8:BF8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BI8:BJ8"/>
+    <mergeCell ref="BK8:BL8"/>
+    <mergeCell ref="BT417:BW417"/>
+    <mergeCell ref="BT418:BW418"/>
+    <mergeCell ref="BT422:BW422"/>
+    <mergeCell ref="BT423:BW423"/>
+    <mergeCell ref="BM8:BN8"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="BQ8:BR8"/>
+    <mergeCell ref="BS8:BV8"/>
+    <mergeCell ref="BW8:BW10"/>
+    <mergeCell ref="BS9:BT9"/>
+    <mergeCell ref="BU9:BV9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.31496062992125984" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>